<commit_message>
Excel Basics ( 17-7-2025 )
</commit_message>
<xml_diff>
--- a/Excel/My-Skill-Set-Track.xlsx
+++ b/Excel/My-Skill-Set-Track.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Data-Analytics\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC725FB9-64BD-481A-9E87-3E5716E22D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851E27CC-AA74-4E6B-9AEF-81BD83CEA754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{1E7A2102-239A-4535-B10C-B1AF6056B40A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Topic</t>
   </si>
@@ -53,7 +54,52 @@
     <t xml:space="preserve">   Date</t>
   </si>
   <si>
-    <t>UI of excel, Quick access, Tabs, Ribbons, Namebox , Formual Bar, Rows, Columns, Cell</t>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Shortcut keys</t>
+  </si>
+  <si>
+    <t>CTRL+Up/Down</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last row and column </t>
+  </si>
+  <si>
+    <t>UI of excel, Quick access, Tabs, Ribbons, Namebox , Formual Bar, Rows, Columns, Cell, Workbook and Worksheets</t>
+  </si>
+  <si>
+    <t>Shift F11</t>
+  </si>
+  <si>
+    <t>add New  Worksheet</t>
+  </si>
+  <si>
+    <t>CTRL pgup/pgdwn</t>
+  </si>
+  <si>
+    <t>Switch Worksheet</t>
+  </si>
+  <si>
+    <t>17-7-2025</t>
+  </si>
+  <si>
+    <t>CTRL + W</t>
+  </si>
+  <si>
+    <t>Close Workbook</t>
+  </si>
+  <si>
+    <t>CTRL+N</t>
+  </si>
+  <si>
+    <t>CTRL+O</t>
+  </si>
+  <si>
+    <t>New  Workbook</t>
+  </si>
+  <si>
+    <t>Open Workbook</t>
   </si>
 </sst>
 </file>
@@ -103,19 +149,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,74 +497,190 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E178CC-A67A-4CEB-9ED6-E0624B3C5E2E}">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:AA11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="1"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="T1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="T2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="W2" s="3"/>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="T3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="W3" s="3"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="T4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="W4" s="3"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="T5" t="s">
+        <v>15</v>
+      </c>
+      <c r="V5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="T6" t="s">
+        <v>17</v>
+      </c>
+      <c r="V6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="W6" s="6"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="T7" t="s">
+        <v>18</v>
+      </c>
+      <c r="V7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="W7" s="6"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="F8">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="F9">
+        <f>55+45</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="F11">
+        <f>F8+F9</f>
+        <v>145</v>
+      </c>
+      <c r="G11">
+        <f>SUM(F8:F9)</f>
+        <v>145</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="D2:M2"/>
+  <mergeCells count="17">
+    <mergeCell ref="V7:W7"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:K1"/>
     <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="D2:N2"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="X1:Y1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E0F8151-937B-4935-B8F3-24E8BCB42125}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Excel Data entry ( 18-7-2025 )
</commit_message>
<xml_diff>
--- a/Excel/My-Skill-Set-Track.xlsx
+++ b/Excel/My-Skill-Set-Track.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Data-Analytics\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851E27CC-AA74-4E6B-9AEF-81BD83CEA754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2FD22B-9F44-4252-9FCC-A107C2EAEAAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{1E7A2102-239A-4535-B10C-B1AF6056B40A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="6" r:id="rId2"/>
+    <sheet name="Practice" sheetId="6" r:id="rId1"/>
+    <sheet name="Track" sheetId="1" r:id="rId2"/>
+    <sheet name="Shorcut Keys" sheetId="7" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Track!$A$1:$AA$3</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Topic</t>
   </si>
@@ -57,9 +61,6 @@
     <t>Action</t>
   </si>
   <si>
-    <t>Shortcut keys</t>
-  </si>
-  <si>
     <t>CTRL+Up/Down</t>
   </si>
   <si>
@@ -81,9 +82,6 @@
     <t>Switch Worksheet</t>
   </si>
   <si>
-    <t>17-7-2025</t>
-  </si>
-  <si>
     <t>CTRL + W</t>
   </si>
   <si>
@@ -100,6 +98,27 @@
   </si>
   <si>
     <t>Open Workbook</t>
+  </si>
+  <si>
+    <t>18-7-2025</t>
+  </si>
+  <si>
+    <t>SUM function, Password Protection on Worksheets and Workbooks</t>
+  </si>
+  <si>
+    <t>Shortcut Keys</t>
+  </si>
+  <si>
+    <t>CTRL+Z</t>
+  </si>
+  <si>
+    <t>CTRL+Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Undo </t>
+  </si>
+  <si>
+    <t>Redo</t>
   </si>
 </sst>
 </file>
@@ -123,7 +142,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,6 +152,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -149,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -162,7 +187,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,11 +525,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E0F8151-937B-4935-B8F3-24E8BCB42125}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.36328125" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E178CC-A67A-4CEB-9ED6-E0624B3C5E2E}">
-  <dimension ref="A1:AA11"/>
+  <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -531,13 +577,9 @@
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
-      <c r="T1" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="T1" s="4"/>
       <c r="U1" s="4"/>
-      <c r="V1" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="V1" s="4"/>
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
@@ -553,7 +595,7 @@
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -565,122 +607,151 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
-      <c r="T2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="W2" s="3"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="T3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="W3" s="3"/>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="T4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="W4" s="3"/>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="T5" t="s">
-        <v>15</v>
-      </c>
-      <c r="V5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="T6" t="s">
-        <v>17</v>
-      </c>
-      <c r="V6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="W6" s="6"/>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="T7" t="s">
-        <v>18</v>
-      </c>
-      <c r="V7" s="6" t="s">
+      <c r="D3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="W7" s="6"/>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="F8">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="F9">
-        <f>55+45</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="F11">
-        <f>F8+F9</f>
-        <v>145</v>
-      </c>
-      <c r="G11">
-        <f>SUM(F8:F9)</f>
-        <v>145</v>
-      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="V7:W7"/>
+  <mergeCells count="10">
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="D2:N2"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="X1:Y1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:K1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="D2:N2"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="D3:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E0F8151-937B-4935-B8F3-24E8BCB42125}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A6F66EB-3F6A-4CB6-B201-8462253FCC87}">
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="9.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="6"/>
+      <c r="B1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="8"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F19" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Learning Basics of Data Entry in Excel ( 21-7-2025 )
</commit_message>
<xml_diff>
--- a/Excel/My-Skill-Set-Track.xlsx
+++ b/Excel/My-Skill-Set-Track.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Data-Analytics\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2FD22B-9F44-4252-9FCC-A107C2EAEAAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97DB57C-E985-4009-8481-E4063EFDC1D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{1E7A2102-239A-4535-B10C-B1AF6056B40A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{1E7A2102-239A-4535-B10C-B1AF6056B40A}"/>
   </bookViews>
   <sheets>
     <sheet name="Practice" sheetId="6" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="111">
   <si>
     <t>Topic</t>
   </si>
@@ -119,13 +119,268 @@
   </si>
   <si>
     <t>Redo</t>
+  </si>
+  <si>
+    <t>SALARY</t>
+  </si>
+  <si>
+    <t>AGE</t>
+  </si>
+  <si>
+    <t>CITY</t>
+  </si>
+  <si>
+    <t>CONTACT NO</t>
+  </si>
+  <si>
+    <t>CTRL+ FILL HANDLE</t>
+  </si>
+  <si>
+    <t>Continue Series eg:( SR NO)</t>
+  </si>
+  <si>
+    <t>EMP0001</t>
+  </si>
+  <si>
+    <t>EMP0002</t>
+  </si>
+  <si>
+    <t>EMP0003</t>
+  </si>
+  <si>
+    <t>EMP0004</t>
+  </si>
+  <si>
+    <t>EMP0005</t>
+  </si>
+  <si>
+    <t>EMP0006</t>
+  </si>
+  <si>
+    <t>EMP0007</t>
+  </si>
+  <si>
+    <t>EMP0008</t>
+  </si>
+  <si>
+    <t>EMP0009</t>
+  </si>
+  <si>
+    <t>EMP0010</t>
+  </si>
+  <si>
+    <t>EMP0011</t>
+  </si>
+  <si>
+    <t>EMP0012</t>
+  </si>
+  <si>
+    <t>EMP0013</t>
+  </si>
+  <si>
+    <t>EMP0014</t>
+  </si>
+  <si>
+    <t>EMP0015</t>
+  </si>
+  <si>
+    <t>EMP0016</t>
+  </si>
+  <si>
+    <t>EMP0017</t>
+  </si>
+  <si>
+    <t>EMP0018</t>
+  </si>
+  <si>
+    <t>EMP0019</t>
+  </si>
+  <si>
+    <t>Karachi</t>
+  </si>
+  <si>
+    <t>Lahore</t>
+  </si>
+  <si>
+    <t>Islamabad</t>
+  </si>
+  <si>
+    <t>Faisalabad</t>
+  </si>
+  <si>
+    <t>Rawalpindi</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>Sukkur</t>
+  </si>
+  <si>
+    <t>EMP ID</t>
+  </si>
+  <si>
+    <t>EMP NAME</t>
+  </si>
+  <si>
+    <t>Haroon Abbas Khan</t>
+  </si>
+  <si>
+    <t>Ali Shaikh</t>
+  </si>
+  <si>
+    <t>Shahzaib Shah</t>
+  </si>
+  <si>
+    <t>Komal Khan</t>
+  </si>
+  <si>
+    <t>Poja Lohana</t>
+  </si>
+  <si>
+    <t>Raimal Raja</t>
+  </si>
+  <si>
+    <t>Talha Arain</t>
+  </si>
+  <si>
+    <t>Faizan Khan</t>
+  </si>
+  <si>
+    <t>Rizwan Shah</t>
+  </si>
+  <si>
+    <t>Dilawar Lashari</t>
+  </si>
+  <si>
+    <t>Akbar Khan</t>
+  </si>
+  <si>
+    <t>Shoquat baloch</t>
+  </si>
+  <si>
+    <t>Sagar Shah</t>
+  </si>
+  <si>
+    <t>Amanat Rehmani</t>
+  </si>
+  <si>
+    <t>Ali Kashmiri</t>
+  </si>
+  <si>
+    <t>Maryam Khan</t>
+  </si>
+  <si>
+    <t>Areeba Tariq</t>
+  </si>
+  <si>
+    <t>Abdul Rehman</t>
+  </si>
+  <si>
+    <t>Zubair Baloch</t>
+  </si>
+  <si>
+    <t>Mirpurkhas</t>
+  </si>
+  <si>
+    <t>Badin</t>
+  </si>
+  <si>
+    <t>Larkhana</t>
+  </si>
+  <si>
+    <t>0349-1233491</t>
+  </si>
+  <si>
+    <t>0349-1233492</t>
+  </si>
+  <si>
+    <t>0349-1233493</t>
+  </si>
+  <si>
+    <t>0349-1233494</t>
+  </si>
+  <si>
+    <t>0349-1233495</t>
+  </si>
+  <si>
+    <t>0349-1233496</t>
+  </si>
+  <si>
+    <t>0349-1233497</t>
+  </si>
+  <si>
+    <t>0349-1233498</t>
+  </si>
+  <si>
+    <t>0349-1233499</t>
+  </si>
+  <si>
+    <t>0349-1233500</t>
+  </si>
+  <si>
+    <t>0349-1233501</t>
+  </si>
+  <si>
+    <t>0349-1233502</t>
+  </si>
+  <si>
+    <t>0349-1233503</t>
+  </si>
+  <si>
+    <t>0349-1233504</t>
+  </si>
+  <si>
+    <t>0349-1233505</t>
+  </si>
+  <si>
+    <t>0349-1233506</t>
+  </si>
+  <si>
+    <t>0349-1233507</t>
+  </si>
+  <si>
+    <t>0349-1233508</t>
+  </si>
+  <si>
+    <t>0349-1233509</t>
+  </si>
+  <si>
+    <t>Double click +Fill handle</t>
+  </si>
+  <si>
+    <t>Fill Column With Data</t>
+  </si>
+  <si>
+    <t>DEPT</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>Operations</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>CTRL+SHIFT+(+)</t>
+  </si>
+  <si>
+    <t>Add New Column</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,6 +392,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -174,23 +435,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -526,17 +800,493 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E0F8151-937B-4935-B8F3-24E8BCB42125}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView zoomScale="90" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.36328125" customWidth="1"/>
+    <col min="2" max="2" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="5.36328125" customWidth="1"/>
+    <col min="7" max="7" width="16.36328125" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="12">
+        <v>38000</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="11">
+        <v>20</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="12">
+        <v>36000</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="11">
+        <v>21</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="12">
+        <v>34000</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="11">
+        <v>21</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="12">
+        <v>32000</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="11">
+        <v>20</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="12">
+        <v>30000</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="11">
+        <v>23</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="12">
+        <v>28000</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="11">
+        <v>24</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="12">
+        <v>26000</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="11">
+        <v>23</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="12">
+        <v>24000</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="11">
+        <v>26</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" s="12">
+        <v>22000</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="11">
+        <v>28</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" s="12">
+        <v>20000</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="11">
+        <v>30</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" s="12">
+        <v>18000</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="11">
+        <v>20</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" s="12">
+        <v>16000</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="11">
+        <v>23</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="12">
+        <v>14000</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" s="11">
+        <v>21</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" s="12">
+        <v>12000</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" s="11">
+        <v>25</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="12">
+        <v>10000</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" s="11">
+        <v>25</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="D17" s="12">
+        <v>8000</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="F17" s="11">
+        <v>21</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" s="12">
+        <v>6000</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="11">
+        <v>20</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="12">
+        <v>4000</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="11">
+        <v>20</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20" s="12">
+        <v>2000</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" s="11">
+        <v>20</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -546,7 +1296,7 @@
   <dimension ref="A1:AA3"/>
   <sheetViews>
     <sheetView zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -590,58 +1340,58 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:K1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:N3"/>
     <mergeCell ref="Z1:AA1"/>
     <mergeCell ref="D2:N2"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:K1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -652,17 +1402,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A6F66EB-3F6A-4CB6-B201-8462253FCC87}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="3" max="3" width="16.7265625" customWidth="1"/>
     <col min="4" max="4" width="9.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="6"/>
+      <c r="A1" s="3"/>
       <c r="B1" s="7" t="s">
         <v>21</v>
       </c>
@@ -671,18 +1422,18 @@
         <v>5</v>
       </c>
       <c r="E1" s="8"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
@@ -728,10 +1479,10 @@
       <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
@@ -741,11 +1492,43 @@
         <v>25</v>
       </c>
     </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B11" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B12" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" t="s">
+        <v>110</v>
+      </c>
+    </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F19" s="6"/>
+      <c r="F19" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="9">
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="D8:E8"/>

</xml_diff>

<commit_message>
Learning Data Entry ( 21-7-2025 )
</commit_message>
<xml_diff>
--- a/Excel/My-Skill-Set-Track.xlsx
+++ b/Excel/My-Skill-Set-Track.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Data-Analytics\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97DB57C-E985-4009-8481-E4063EFDC1D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9110047C-E905-483F-BCFD-D05E8BEB3909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{1E7A2102-239A-4535-B10C-B1AF6056B40A}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="115">
   <si>
     <t>Topic</t>
   </si>
@@ -373,7 +373,19 @@
     <t>CTRL+SHIFT+(+)</t>
   </si>
   <si>
-    <t>Add New Column</t>
+    <t>CTRL+(-)</t>
+  </si>
+  <si>
+    <t>Add New Column or Row</t>
+  </si>
+  <si>
+    <t>Delete Column or Row</t>
+  </si>
+  <si>
+    <t>Cell + (+)</t>
+  </si>
+  <si>
+    <t>DialogBox to chose what to add</t>
   </si>
 </sst>
 </file>
@@ -403,7 +415,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -422,6 +434,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -435,7 +453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -466,6 +484,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,7 +822,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1403,7 +1422,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1516,15 +1535,41 @@
         <v>109</v>
       </c>
       <c r="C12" s="13"/>
-      <c r="D12" t="s">
+      <c r="D12" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B13" s="5" t="s">
         <v>110</v>
       </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F19" s="3"/>
+      <c r="F19" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="13">
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:F14"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:E11"/>

</xml_diff>

<commit_message>
Learning Data Entry ( 22-7-2025 )
</commit_message>
<xml_diff>
--- a/Excel/My-Skill-Set-Track.xlsx
+++ b/Excel/My-Skill-Set-Track.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Data-Analytics\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9110047C-E905-483F-BCFD-D05E8BEB3909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F9ADD3-2C81-463F-A909-0A8ACE3DE37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{1E7A2102-239A-4535-B10C-B1AF6056B40A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{1E7A2102-239A-4535-B10C-B1AF6056B40A}"/>
   </bookViews>
   <sheets>
     <sheet name="Practice" sheetId="6" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="141">
   <si>
     <t>Topic</t>
   </si>
@@ -386,13 +386,95 @@
   </si>
   <si>
     <t>DialogBox to chose what to add</t>
+  </si>
+  <si>
+    <t>20-7-2025</t>
+  </si>
+  <si>
+    <t>Data Entry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fill handle, Filling Columns , adding Columns , row , Deleting Columns , rows  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">21-7-2025 </t>
+  </si>
+  <si>
+    <t>CTRL+1</t>
+  </si>
+  <si>
+    <t>Open Number Format</t>
+  </si>
+  <si>
+    <t>JOINING DATE</t>
+  </si>
+  <si>
+    <t>To select complete column to appy formula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTRL+SHIFT + UP or DOWN </t>
+  </si>
+  <si>
+    <t>To control Selection for formulas</t>
+  </si>
+  <si>
+    <t>SHIFT  + UP or DOWN</t>
+  </si>
+  <si>
+    <t>Adding Borders, Formating Borders,Number Format,Date Format, Column Selection  for formulas</t>
+  </si>
+  <si>
+    <t>SUB1</t>
+  </si>
+  <si>
+    <t>SUB2</t>
+  </si>
+  <si>
+    <t>SUB3</t>
+  </si>
+  <si>
+    <t>CTRL +R</t>
+  </si>
+  <si>
+    <t>Fill Right</t>
+  </si>
+  <si>
+    <t>CTRL + D</t>
+  </si>
+  <si>
+    <t>Fill Down</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>ALT+=</t>
+  </si>
+  <si>
+    <t>SUM ROW</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>To Fix Value in Formula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22-7-2025 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUM Formula , adding marks </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="dd\-mmm\-yyyy"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -410,6 +492,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -441,7 +530,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -449,21 +538,64 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -471,22 +603,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -819,10 +942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E0F8151-937B-4935-B8F3-24E8BCB42125}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -830,479 +953,691 @@
     <col min="1" max="1" width="9.36328125" customWidth="1"/>
     <col min="2" max="2" width="18.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.453125" customWidth="1"/>
-    <col min="4" max="4" width="12.1796875" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" style="16" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
     <col min="6" max="6" width="5.36328125" customWidth="1"/>
     <col min="7" max="7" width="16.36328125" customWidth="1"/>
+    <col min="8" max="8" width="14.7265625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:15" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="H1" s="11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="14">
         <v>38000</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="7">
         <v>20</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="7" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="H2" s="12">
+        <v>45661</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="14">
         <v>36000</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="7">
         <v>21</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="7" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="H3" s="12">
+        <v>45662</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="14">
         <v>34000</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="7">
         <v>21</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="7" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="H4" s="12">
+        <v>45663</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="14">
         <v>32000</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="7">
         <v>20</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="7" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="H5" s="12">
+        <v>45664</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="14">
         <v>30000</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="7">
         <v>23</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="7" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="H6" s="12">
+        <v>45665</v>
+      </c>
+      <c r="L6" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="M6" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="N6" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="O6" s="23" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="14">
         <v>28000</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="7">
         <v>24</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="7" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="H7" s="12">
+        <v>45666</v>
+      </c>
+      <c r="L7">
+        <v>85</v>
+      </c>
+      <c r="M7">
+        <v>37</v>
+      </c>
+      <c r="N7">
+        <v>25</v>
+      </c>
+      <c r="O7">
+        <f>SUM(L7:N7)+$L$19</f>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="14">
         <v>26000</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="7">
         <v>23</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="7" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="H8" s="12">
+        <v>45667</v>
+      </c>
+      <c r="L8">
+        <v>48</v>
+      </c>
+      <c r="M8">
+        <v>18</v>
+      </c>
+      <c r="N8">
+        <v>48</v>
+      </c>
+      <c r="O8">
+        <f t="shared" ref="O8:O16" si="0">SUM(L8:N8)+$L$19</f>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="14">
         <v>24000</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="7">
         <v>26</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="7" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="H9" s="12">
+        <v>45668</v>
+      </c>
+      <c r="L9">
+        <v>39</v>
+      </c>
+      <c r="M9">
+        <v>72</v>
+      </c>
+      <c r="N9">
+        <v>58</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="14">
         <v>22000</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="7">
         <v>28</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="7" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="H10" s="12">
+        <v>45669</v>
+      </c>
+      <c r="L10">
+        <v>29</v>
+      </c>
+      <c r="M10">
+        <v>40</v>
+      </c>
+      <c r="N10">
+        <v>49</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="14">
         <v>20000</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="7">
         <v>30</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="7" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="H11" s="12">
+        <v>45670</v>
+      </c>
+      <c r="L11">
+        <v>74</v>
+      </c>
+      <c r="M11">
+        <v>99</v>
+      </c>
+      <c r="N11">
+        <v>70</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>253</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="14">
         <v>18000</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="7">
         <v>20</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="7" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="H12" s="12">
+        <v>45671</v>
+      </c>
+      <c r="L12">
+        <v>32</v>
+      </c>
+      <c r="M12">
+        <v>81</v>
+      </c>
+      <c r="N12">
+        <v>26</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="14">
         <v>16000</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="7">
         <v>23</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="7" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="H13" s="12">
+        <v>45672</v>
+      </c>
+      <c r="L13">
+        <v>49</v>
+      </c>
+      <c r="M13">
+        <v>47</v>
+      </c>
+      <c r="N13">
+        <v>94</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="14">
         <v>14000</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="7">
         <v>21</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="7" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="H14" s="12">
+        <v>45673</v>
+      </c>
+      <c r="L14">
+        <v>46</v>
+      </c>
+      <c r="M14">
+        <v>29</v>
+      </c>
+      <c r="N14">
+        <v>93</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="0"/>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="14">
         <v>12000</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="7">
         <v>25</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="7" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="H15" s="12">
+        <v>45674</v>
+      </c>
+      <c r="L15">
+        <v>94</v>
+      </c>
+      <c r="M15">
+        <v>4</v>
+      </c>
+      <c r="N15">
+        <v>51</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="0"/>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="14">
         <v>10000</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="7">
         <v>25</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="7" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="H16" s="12">
+        <v>45675</v>
+      </c>
+      <c r="L16">
+        <v>52</v>
+      </c>
+      <c r="M16">
+        <v>75</v>
+      </c>
+      <c r="N16">
+        <v>31</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="0"/>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="14">
         <v>8000</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="7">
         <v>21</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="7" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="H17" s="12">
+        <v>45676</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="14">
         <v>6000</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="7">
         <v>20</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="7" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="H18" s="12">
+        <v>45677</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D19" s="14">
         <v>4000</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="7">
         <v>20</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="G19" s="7" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="H19" s="12">
+        <v>45678</v>
+      </c>
+      <c r="L19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20" s="14">
         <v>2000</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="7">
         <v>20</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="7" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
+      <c r="H20" s="12">
+        <v>45679</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="15">
+        <f>SUM(D2:D20)</f>
+        <v>380000</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C23" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1312,32 +1647,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E178CC-A67A-4CEB-9ED6-E0624B3C5E2E}">
-  <dimension ref="A1:AA3"/>
+  <dimension ref="A1:AA6"/>
   <sheetViews>
-    <sheetView zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.54296875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="2"/>
@@ -1346,71 +1684,124 @@
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="18"/>
+      <c r="AA1" s="18"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="17"/>
+      <c r="D3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" t="s">
+        <v>140</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="13">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:J4"/>
+    <mergeCell ref="D5:N5"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="D2:N2"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="X1:Y1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:K1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D3:N3"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="D2:N2"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="X1:Y1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1419,10 +1810,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A6F66EB-3F6A-4CB6-B201-8462253FCC87}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1431,30 +1822,30 @@
     <col min="4" max="4" width="9.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="3"/>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="8" t="s">
+      <c r="C1" s="20"/>
+      <c r="D1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="8"/>
+      <c r="E1" s="21"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E2" s="17"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>9</v>
       </c>
@@ -1462,7 +1853,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -1470,7 +1861,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>13</v>
       </c>
@@ -1478,7 +1869,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>15</v>
       </c>
@@ -1486,7 +1877,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>16</v>
       </c>
@@ -1494,16 +1885,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E8" s="17"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>23</v>
       </c>
@@ -1511,61 +1902,131 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B10" s="5" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B10" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="17"/>
       <c r="D10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B11" s="5" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B11" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5" t="s">
+      <c r="C11" s="17"/>
+      <c r="D11" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B12" s="13" t="s">
+      <c r="E11" s="17"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B12" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="5" t="s">
+      <c r="C12" s="22"/>
+      <c r="D12" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B13" s="5" t="s">
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B13" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5" t="s">
+      <c r="C13" s="17"/>
+      <c r="D13" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E13" s="17"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>113</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F19" s="14"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>119</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B16" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B17" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>130</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D19" t="s">
+        <v>133</v>
+      </c>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>135</v>
+      </c>
+      <c r="D20" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>137</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="E21" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="20">
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D21:E21"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="D13:E13"/>
@@ -1579,6 +2040,11 @@
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:H16"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Completed Data Entry(23-7-2025 )
</commit_message>
<xml_diff>
--- a/Excel/My-Skill-Set-Track.xlsx
+++ b/Excel/My-Skill-Set-Track.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Data-Analytics\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617498E0-80BF-47F2-A6DF-2031228978CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9A5DA4-BE7C-4FDB-A963-911BB15B3FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{1E7A2102-239A-4535-B10C-B1AF6056B40A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{1E7A2102-239A-4535-B10C-B1AF6056B40A}"/>
   </bookViews>
   <sheets>
     <sheet name="Practice" sheetId="6" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="147">
   <si>
     <t>Topic</t>
   </si>
@@ -476,6 +476,12 @@
   </si>
   <si>
     <t>SUM Formula , adding marks ,paste values, fix refrence , relative refrence,MAX,MIN,AVG,COUNT</t>
+  </si>
+  <si>
+    <t>23-7-2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conditional Formating,Advance Conditional Formating </t>
   </si>
 </sst>
 </file>
@@ -624,8 +630,75 @@
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDF240"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDF240"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDF240"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFDDF240"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -956,8 +1029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E0F8151-937B-4935-B8F3-24E8BCB42125}">
   <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" zoomScale="90" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView zoomScale="90" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1258,7 +1331,7 @@
         <v>38</v>
       </c>
       <c r="S8">
-        <f t="shared" ref="S8:S16" si="4">COUNT(L8:N8)</f>
+        <f t="shared" ref="S8:S15" si="4">COUNT(L8:N8)</f>
         <v>3</v>
       </c>
     </row>
@@ -1812,10 +1885,7 @@
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
-      <c r="D21" s="15">
-        <f>SUM(D2:D20)</f>
-        <v>380000</v>
-      </c>
+      <c r="D21" s="15"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -1825,21 +1895,27 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="A2:H20">
+    <cfRule type="expression" dxfId="5" priority="2">
+      <formula>$C2="IT"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E178CC-A67A-4CEB-9ED6-E0624B3C5E2E}">
-  <dimension ref="A1:AA6"/>
+  <dimension ref="A1:AA7"/>
   <sheetViews>
     <sheetView zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="F18" activeCellId="1" sqref="D6:L6 F18"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.54296875" customWidth="1"/>
+    <col min="4" max="4" width="95.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.35">
@@ -1978,6 +2054,17 @@
       <c r="J6" s="18"/>
       <c r="K6" s="18"/>
       <c r="L6" s="18"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D7" t="s">
+        <v>146</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -2005,7 +2092,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A6F66EB-3F6A-4CB6-B201-8462253FCC87}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -2218,15 +2305,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
     <mergeCell ref="D18:F18"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="B13:C13"/>
@@ -2238,6 +2316,15 @@
     <mergeCell ref="D16:H16"/>
     <mergeCell ref="D17:G17"/>
     <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Solving Practice Problems ( 23-7-2025 )
</commit_message>
<xml_diff>
--- a/Excel/My-Skill-Set-Track.xlsx
+++ b/Excel/My-Skill-Set-Track.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Data-Analytics\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9A5DA4-BE7C-4FDB-A963-911BB15B3FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EAA5D92-34E2-4D95-9CDD-1F7D4840788C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{1E7A2102-239A-4535-B10C-B1AF6056B40A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{1E7A2102-239A-4535-B10C-B1AF6056B40A}"/>
   </bookViews>
   <sheets>
     <sheet name="Practice" sheetId="6" r:id="rId1"/>
-    <sheet name="Track" sheetId="1" r:id="rId2"/>
-    <sheet name="Shorcut Keys" sheetId="7" r:id="rId3"/>
+    <sheet name="Practice Problems" sheetId="8" r:id="rId2"/>
+    <sheet name="Track" sheetId="1" r:id="rId3"/>
+    <sheet name="Shorcut Keys" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Track!$A$1:$AA$3</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">Track!$A$1:$AA$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="171">
   <si>
     <t>Topic</t>
   </si>
@@ -482,6 +483,78 @@
   </si>
   <si>
     <t xml:space="preserve">Conditional Formating,Advance Conditional Formating </t>
+  </si>
+  <si>
+    <t>EMP0020</t>
+  </si>
+  <si>
+    <t>Zeeshan</t>
+  </si>
+  <si>
+    <t>0349-1233510</t>
+  </si>
+  <si>
+    <t>23/1/2025</t>
+  </si>
+  <si>
+    <t>ALT+D+0</t>
+  </si>
+  <si>
+    <t>Activate Data Entry Form</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <t>Science</t>
+  </si>
+  <si>
+    <t>Ali</t>
+  </si>
+  <si>
+    <t>Sara</t>
+  </si>
+  <si>
+    <t>Bilal</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Highest: </t>
+  </si>
+  <si>
+    <t>Avg:</t>
+  </si>
+  <si>
+    <t>&gt;80</t>
+  </si>
+  <si>
+    <t>Haroon</t>
+  </si>
+  <si>
+    <t>Shan</t>
+  </si>
+  <si>
+    <t>Suleman</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Running Total</t>
+  </si>
+  <si>
+    <t>Count</t>
   </si>
 </sst>
 </file>
@@ -548,7 +621,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -571,21 +644,98 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -606,9 +756,6 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -625,70 +772,43 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFDDF240"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDDF240"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDDF240"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1030,7 +1150,7 @@
   <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1038,216 +1158,216 @@
     <col min="1" max="1" width="9.36328125" customWidth="1"/>
     <col min="2" max="2" width="18.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.453125" customWidth="1"/>
-    <col min="4" max="4" width="12.1796875" style="16" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" style="14" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
     <col min="6" max="6" width="5.36328125" customWidth="1"/>
     <col min="7" max="7" width="16.36328125" customWidth="1"/>
-    <col min="8" max="8" width="14.7265625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="14.7265625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="13">
         <v>38000</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <v>20</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="H2" s="12">
+      <c r="H2" s="11">
         <v>45661</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="13">
         <v>36000</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="6">
         <v>21</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="11">
         <v>45662</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="13">
         <v>34000</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="6">
         <v>21</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="11">
         <v>45663</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="13">
         <v>32000</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <v>20</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="11">
         <v>45664</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="13">
         <v>30000</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <v>23</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="11">
         <v>45665</v>
       </c>
-      <c r="L6" s="17" t="s">
+      <c r="L6" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="M6" s="17" t="s">
+      <c r="M6" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="N6" s="17" t="s">
+      <c r="N6" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="O6" s="17" t="s">
+      <c r="O6" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="P6" s="17" t="s">
+      <c r="P6" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="Q6" s="17" t="s">
+      <c r="Q6" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="R6" s="17" t="s">
+      <c r="R6" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="S6" s="17" t="s">
+      <c r="S6" s="15" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="13">
         <v>28000</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <v>24</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="11">
         <v>45666</v>
       </c>
       <c r="L7">
@@ -1281,28 +1401,28 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="13">
         <v>26000</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <v>23</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="11">
         <v>45667</v>
       </c>
       <c r="L8">
@@ -1336,28 +1456,28 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="13">
         <v>24000</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <v>26</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="11">
         <v>45668</v>
       </c>
       <c r="L9">
@@ -1391,28 +1511,28 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="13">
         <v>22000</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="6">
         <v>28</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="11">
         <v>45669</v>
       </c>
       <c r="L10">
@@ -1446,28 +1566,28 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="13">
         <v>20000</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <v>30</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="11">
         <v>45670</v>
       </c>
       <c r="L11">
@@ -1501,28 +1621,28 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="13">
         <v>18000</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <v>20</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="11">
         <v>45671</v>
       </c>
       <c r="L12">
@@ -1556,28 +1676,28 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="13">
         <v>16000</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="6">
         <v>23</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="11">
         <v>45672</v>
       </c>
       <c r="L13">
@@ -1611,28 +1731,28 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="13">
         <v>14000</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="6">
         <v>21</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="11">
         <v>45673</v>
       </c>
       <c r="L14">
@@ -1666,28 +1786,28 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="13">
         <v>12000</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="6">
         <v>25</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="11">
         <v>45674</v>
       </c>
       <c r="L15">
@@ -1721,28 +1841,28 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16" s="13">
         <v>10000</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="6">
         <v>25</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G16" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="11">
         <v>45675</v>
       </c>
       <c r="L16">
@@ -1776,80 +1896,80 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="13">
         <v>8000</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="6">
         <v>21</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="11">
         <v>45676</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="13">
         <v>6000</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="6">
         <v>20</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="H18" s="12">
+      <c r="H18" s="11">
         <v>45677</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="13">
         <v>4000</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="6">
         <v>20</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G19" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="H19" s="12">
+      <c r="H19" s="11">
         <v>45678</v>
       </c>
       <c r="L19">
@@ -1857,46 +1977,64 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="13">
         <v>2000</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="6">
         <v>20</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="H20" s="12">
+      <c r="H20" s="11">
         <v>45679</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
+      <c r="A21" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21" s="13">
+        <v>2000</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F21" s="6">
+        <v>28</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="C23" s="5"/>
+      <c r="C23" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A2:H20">
-    <cfRule type="expression" dxfId="5" priority="2">
+  <conditionalFormatting sqref="A2:H22">
+    <cfRule type="expression" dxfId="0" priority="10">
       <formula>$C2="IT"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1905,6 +2043,279 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E13B64D4-A1D5-4271-9163-F4CC547F860B}">
+  <dimension ref="A1:I16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" s="24">
+        <v>78</v>
+      </c>
+      <c r="C2" s="24">
+        <v>83</v>
+      </c>
+      <c r="D2" s="24">
+        <v>91</v>
+      </c>
+      <c r="E2" s="25">
+        <f>SUM(B2:D2)</f>
+        <v>252</v>
+      </c>
+      <c r="F2" s="25">
+        <f>MAX(B2:D2)</f>
+        <v>91</v>
+      </c>
+      <c r="G2" s="25">
+        <f>MIN(B2:D2)</f>
+        <v>78</v>
+      </c>
+      <c r="H2" s="25">
+        <f>AVERAGE(B2:D2)</f>
+        <v>84</v>
+      </c>
+      <c r="I2" s="26">
+        <f>COUNT(B2:D2)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" s="28">
+        <v>65</v>
+      </c>
+      <c r="C3" s="28">
+        <v>74</v>
+      </c>
+      <c r="D3" s="28">
+        <v>88</v>
+      </c>
+      <c r="E3" s="29">
+        <f t="shared" ref="E3:E7" si="0">SUM(B3:D3)</f>
+        <v>227</v>
+      </c>
+      <c r="F3" s="29">
+        <f t="shared" ref="F3:F7" si="1">MAX(B3:D3)</f>
+        <v>88</v>
+      </c>
+      <c r="G3" s="29">
+        <f t="shared" ref="G3:G7" si="2">MIN(B3:D3)</f>
+        <v>65</v>
+      </c>
+      <c r="H3" s="29">
+        <f t="shared" ref="H3:H7" si="3">AVERAGE(B3:D3)</f>
+        <v>75.666666666666671</v>
+      </c>
+      <c r="I3" s="30">
+        <f t="shared" ref="I3:I7" si="4">COUNT(B3:D3)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" s="28">
+        <v>90</v>
+      </c>
+      <c r="C4" s="28">
+        <v>80</v>
+      </c>
+      <c r="D4" s="28">
+        <v>85</v>
+      </c>
+      <c r="E4" s="29">
+        <f t="shared" si="0"/>
+        <v>255</v>
+      </c>
+      <c r="F4" s="29">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="G4" s="29">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="H4" s="29">
+        <f t="shared" si="3"/>
+        <v>85</v>
+      </c>
+      <c r="I4" s="30">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="B5" s="28">
+        <v>64</v>
+      </c>
+      <c r="C5" s="28">
+        <v>94</v>
+      </c>
+      <c r="D5" s="28">
+        <v>77</v>
+      </c>
+      <c r="E5" s="29">
+        <f t="shared" si="0"/>
+        <v>235</v>
+      </c>
+      <c r="F5" s="29">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="G5" s="29">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="H5" s="29">
+        <f t="shared" si="3"/>
+        <v>78.333333333333329</v>
+      </c>
+      <c r="I5" s="30">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="B6" s="28">
+        <v>84</v>
+      </c>
+      <c r="C6" s="28">
+        <v>42</v>
+      </c>
+      <c r="D6" s="28">
+        <v>92</v>
+      </c>
+      <c r="E6" s="29">
+        <f t="shared" si="0"/>
+        <v>218</v>
+      </c>
+      <c r="F6" s="29">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="G6" s="29">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="H6" s="29">
+        <f t="shared" si="3"/>
+        <v>72.666666666666671</v>
+      </c>
+      <c r="I6" s="30">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="B7" s="32">
+        <v>43</v>
+      </c>
+      <c r="C7" s="32">
+        <v>53</v>
+      </c>
+      <c r="D7" s="32">
+        <v>84</v>
+      </c>
+      <c r="E7" s="33">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="F7" s="33">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="G7" s="33">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="H7" s="33">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="I7" s="34">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>163</v>
+      </c>
+      <c r="C15" t="s">
+        <v>161</v>
+      </c>
+      <c r="D15" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B16">
+        <f>COUNTIF(B2:B7,"&gt;80")</f>
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <f>MAX(C2:C7)</f>
+        <v>94</v>
+      </c>
+      <c r="D16">
+        <f>AVERAGE(D2:D7)</f>
+        <v>86.166666666666671</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E178CC-A67A-4CEB-9ED6-E0624B3C5E2E}">
   <dimension ref="A1:AA7"/>
   <sheetViews>
@@ -1922,20 +2333,20 @@
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="2"/>
@@ -1944,76 +2355,76 @@
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="19"/>
-      <c r="Z1" s="19"/>
-      <c r="AA1" s="19"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="17"/>
+      <c r="AA1" s="17"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="18" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18" t="s">
+      <c r="C3" s="16"/>
+      <c r="D3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18" t="s">
+      <c r="C4" s="16"/>
+      <c r="D4" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -2022,19 +2433,19 @@
       <c r="B5" t="s">
         <v>116</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -2043,17 +2454,17 @@
       <c r="B6" t="s">
         <v>116</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -2088,42 +2499,42 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A6F66EB-3F6A-4CB6-B201-8462253FCC87}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="16.7265625" customWidth="1"/>
-    <col min="4" max="4" width="9.54296875" customWidth="1"/>
+    <col min="4" max="4" width="44" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="3"/>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="23" t="s">
+      <c r="C1" s="20"/>
+      <c r="D1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="23"/>
+      <c r="E1" s="21"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="18"/>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
@@ -2169,10 +2580,10 @@
       <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="18"/>
+      <c r="E8" s="16"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
@@ -2183,99 +2594,99 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="18"/>
+      <c r="C10" s="16"/>
       <c r="D10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18" t="s">
+      <c r="C11" s="16"/>
+      <c r="D11" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="E11" s="18"/>
+      <c r="E11" s="16"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="18" t="s">
+      <c r="C12" s="19"/>
+      <c r="D12" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18" t="s">
+      <c r="C13" s="16"/>
+      <c r="D13" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="E13" s="18"/>
+      <c r="E13" s="16"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>113</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>119</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18" t="s">
+      <c r="C16" s="16"/>
+      <c r="D16" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18" t="s">
+      <c r="C17" s="16"/>
+      <c r="D17" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>130</v>
       </c>
-      <c r="D18" s="18" t="s">
+      <c r="D18" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
@@ -2284,7 +2695,7 @@
       <c r="D19" t="s">
         <v>133</v>
       </c>
-      <c r="F19" s="5"/>
+      <c r="F19" s="4"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
@@ -2298,10 +2709,18 @@
       <c r="B21" t="s">
         <v>137</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="D21" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="E21" s="18"/>
+      <c r="E21" s="16"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>151</v>
+      </c>
+      <c r="D22" t="s">
+        <v>152</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="20">

</xml_diff>

<commit_message>
Practice ( 24-7-2025 )
</commit_message>
<xml_diff>
--- a/Excel/My-Skill-Set-Track.xlsx
+++ b/Excel/My-Skill-Set-Track.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Data-Analytics\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EAA5D92-34E2-4D95-9CDD-1F7D4840788C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB4BEBC-E965-4A95-A84C-5A4583997337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{1E7A2102-239A-4535-B10C-B1AF6056B40A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{1E7A2102-239A-4535-B10C-B1AF6056B40A}"/>
   </bookViews>
   <sheets>
     <sheet name="Practice" sheetId="6" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="184">
   <si>
     <t>Topic</t>
   </si>
@@ -545,22 +545,61 @@
     <t>Suleman</t>
   </si>
   <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
+    <t>TEST DATE</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>February</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>December</t>
+  </si>
+  <si>
+    <t>Urdu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24-7-2025 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Practice </t>
+  </si>
+  <si>
+    <t>Solving Problems</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="dd\-mmm\-yyyy"/>
@@ -621,7 +660,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -645,83 +684,132 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thick">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="dotted">
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -729,7 +817,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -758,6 +846,36 @@
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -772,39 +890,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -812,8 +910,222 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dotted">
+          <color indexed="64"/>
+        </left>
+        <right style="thick">
+          <color indexed="64"/>
+        </right>
+        <top style="dotted">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dotted">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dotted">
+          <color indexed="64"/>
+        </left>
+        <right style="dotted">
+          <color indexed="64"/>
+        </right>
+        <top style="dotted">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dotted">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dotted">
+          <color indexed="64"/>
+        </left>
+        <right style="dotted">
+          <color indexed="64"/>
+        </right>
+        <top style="dotted">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dotted">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dotted">
+          <color indexed="64"/>
+        </left>
+        <right style="dotted">
+          <color indexed="64"/>
+        </right>
+        <top style="dotted">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dotted">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dotted">
+          <color indexed="64"/>
+        </left>
+        <right style="dotted">
+          <color indexed="64"/>
+        </right>
+        <top style="dotted">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dotted">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dotted">
+          <color indexed="64"/>
+        </left>
+        <right style="dotted">
+          <color indexed="64"/>
+        </right>
+        <top style="dotted">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dotted">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dotted">
+          <color indexed="64"/>
+        </left>
+        <right style="dotted">
+          <color indexed="64"/>
+        </right>
+        <top style="dotted">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dotted">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dotted">
+          <color indexed="64"/>
+        </left>
+        <right style="dotted">
+          <color indexed="64"/>
+        </right>
+        <top style="dotted">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dotted">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dotted">
+          <color indexed="64"/>
+        </left>
+        <right style="dotted">
+          <color indexed="64"/>
+        </right>
+        <top style="dotted">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dotted">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color indexed="64"/>
+        </left>
+        <right style="dotted">
+          <color indexed="64"/>
+        </right>
+        <top style="dotted">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dotted">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Table Style 1" pivot="0" count="0" xr9:uid="{F2F35C44-564F-4823-B367-B7896C0D6AD3}"/>
+  </tableStyles>
   <colors>
     <mruColors>
       <color rgb="FFDDF240"/>
@@ -828,6 +1140,46 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{23555376-2007-4736-A2FA-A02677D80CA8}" name="Table5" displayName="Table5" ref="A1:J7" totalsRowShown="0" headerRowDxfId="13" tableBorderDxfId="12">
+  <autoFilter ref="A1:J7" xr:uid="{23555376-2007-4736-A2FA-A02677D80CA8}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
+    <filterColumn colId="9" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{DBFED875-5164-47DB-BA0D-B3545E7599AC}" name="Name" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{ED7E621D-B0E7-4E0F-AE49-87626254BEDD}" name="English" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{914CB95C-B4D4-4666-8731-AE771C9B8054}" name="Urdu" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{482F1B75-C013-4781-A7DC-7C06683CBD73}" name="Math" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{A2EB3CEA-91E6-4D55-B25B-F7F6AA16E0F3}" name="Science" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{AF8D4C8A-4FA8-4CD6-AA02-F79836D18D49}" name="SUM" dataDxfId="6">
+      <calculatedColumnFormula>SUM(B2:E2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{7C01B78E-31E9-468C-9645-53B25733C019}" name="MAX" dataDxfId="5">
+      <calculatedColumnFormula>MAX(B2:E2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{3531EF90-C0D8-425F-8DD9-541D509B8B73}" name="MIN" dataDxfId="4">
+      <calculatedColumnFormula>MIN(B2:E2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{C539E7AC-D3A5-4230-9E8A-5F7472DD348E}" name="AVG" dataDxfId="3">
+      <calculatedColumnFormula>AVERAGE(B2:E2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{CE9690EC-BB92-49C8-A5B5-A7E5A3110BE3}" name="COUNT" dataDxfId="2">
+      <calculatedColumnFormula>COUNT(B2:E2)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2034,7 +2386,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A2:H22">
-    <cfRule type="expression" dxfId="0" priority="10">
+    <cfRule type="expression" dxfId="1" priority="10">
       <formula>$C2="IT"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2044,283 +2396,409 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E13B64D4-A1D5-4271-9163-F4CC547F860B}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="3" width="8.90625" customWidth="1"/>
+    <col min="5" max="5" width="9.54296875" customWidth="1"/>
+    <col min="10" max="10" width="8.81640625" customWidth="1"/>
+    <col min="12" max="12" width="11" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:14" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="E1" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="F1" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="G1" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="H1" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="I1" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="J1" s="16" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="23" t="s">
+      <c r="L1" s="16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="24">
+      <c r="B2" s="18">
         <v>78</v>
       </c>
-      <c r="C2" s="24">
+      <c r="C2" s="18">
+        <v>56</v>
+      </c>
+      <c r="D2" s="18">
         <v>83</v>
       </c>
-      <c r="D2" s="24">
+      <c r="E2" s="18">
         <v>91</v>
       </c>
-      <c r="E2" s="25">
-        <f>SUM(B2:D2)</f>
-        <v>252</v>
-      </c>
-      <c r="F2" s="25">
-        <f>MAX(B2:D2)</f>
+      <c r="F2" s="19">
+        <f>SUM(B2:E2)</f>
+        <v>308</v>
+      </c>
+      <c r="G2" s="19">
+        <f>MAX(B2:E2)</f>
         <v>91</v>
       </c>
-      <c r="G2" s="25">
-        <f>MIN(B2:D2)</f>
-        <v>78</v>
-      </c>
-      <c r="H2" s="25">
-        <f>AVERAGE(B2:D2)</f>
-        <v>84</v>
-      </c>
-      <c r="I2" s="26">
-        <f>COUNT(B2:D2)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="27" t="s">
+      <c r="H2" s="19">
+        <f>MIN(B2:E2)</f>
+        <v>56</v>
+      </c>
+      <c r="I2" s="25">
+        <f>AVERAGE(B2:E2)</f>
+        <v>77</v>
+      </c>
+      <c r="J2" s="20">
+        <f>COUNT(B2:E2)</f>
+        <v>4</v>
+      </c>
+      <c r="L2" s="9">
+        <v>45658</v>
+      </c>
+      <c r="N2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="28">
+      <c r="B3" s="22">
         <v>65</v>
       </c>
-      <c r="C3" s="28">
+      <c r="C3" s="22">
         <v>74</v>
       </c>
-      <c r="D3" s="28">
+      <c r="D3" s="22">
+        <v>74</v>
+      </c>
+      <c r="E3" s="22">
         <v>88</v>
       </c>
-      <c r="E3" s="29">
-        <f t="shared" ref="E3:E7" si="0">SUM(B3:D3)</f>
-        <v>227</v>
-      </c>
-      <c r="F3" s="29">
-        <f t="shared" ref="F3:F7" si="1">MAX(B3:D3)</f>
+      <c r="F3" s="23">
+        <f t="shared" ref="F3:F7" si="0">SUM(B3:E3)</f>
+        <v>301</v>
+      </c>
+      <c r="G3" s="23">
+        <f t="shared" ref="G3:G7" si="1">MAX(B3:E3)</f>
         <v>88</v>
       </c>
-      <c r="G3" s="29">
-        <f t="shared" ref="G3:G7" si="2">MIN(B3:D3)</f>
+      <c r="H3" s="23">
+        <f t="shared" ref="H3:H7" si="2">MIN(B3:E3)</f>
         <v>65</v>
       </c>
-      <c r="H3" s="29">
-        <f t="shared" ref="H3:H7" si="3">AVERAGE(B3:D3)</f>
-        <v>75.666666666666671</v>
-      </c>
-      <c r="I3" s="30">
-        <f t="shared" ref="I3:I7" si="4">COUNT(B3:D3)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="27" t="s">
+      <c r="I3" s="26">
+        <f t="shared" ref="I3:I7" si="3">AVERAGE(B3:E3)</f>
+        <v>75.25</v>
+      </c>
+      <c r="J3" s="24">
+        <f t="shared" ref="J3:J7" si="4">COUNT(B3:E3)</f>
+        <v>4</v>
+      </c>
+      <c r="L3" s="9">
+        <v>45658</v>
+      </c>
+      <c r="N3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="22">
         <v>90</v>
       </c>
-      <c r="C4" s="28">
+      <c r="C4" s="22">
+        <v>93</v>
+      </c>
+      <c r="D4" s="22">
         <v>80</v>
       </c>
-      <c r="D4" s="28">
+      <c r="E4" s="22">
         <v>85</v>
       </c>
-      <c r="E4" s="29">
+      <c r="F4" s="23">
         <f t="shared" si="0"/>
-        <v>255</v>
-      </c>
-      <c r="F4" s="29">
+        <v>348</v>
+      </c>
+      <c r="G4" s="23">
         <f t="shared" si="1"/>
-        <v>90</v>
-      </c>
-      <c r="G4" s="29">
+        <v>93</v>
+      </c>
+      <c r="H4" s="23">
         <f t="shared" si="2"/>
         <v>80</v>
       </c>
-      <c r="H4" s="29">
+      <c r="I4" s="26">
         <f t="shared" si="3"/>
-        <v>85</v>
-      </c>
-      <c r="I4" s="30">
+        <v>87</v>
+      </c>
+      <c r="J4" s="24">
         <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4" s="9">
+        <v>45658</v>
+      </c>
+      <c r="N4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="22">
         <v>64</v>
       </c>
-      <c r="C5" s="28">
+      <c r="C5" s="22">
+        <v>67</v>
+      </c>
+      <c r="D5" s="22">
         <v>94</v>
       </c>
-      <c r="D5" s="28">
+      <c r="E5" s="22">
         <v>77</v>
       </c>
-      <c r="E5" s="29">
+      <c r="F5" s="23">
         <f t="shared" si="0"/>
-        <v>235</v>
-      </c>
-      <c r="F5" s="29">
+        <v>302</v>
+      </c>
+      <c r="G5" s="23">
         <f t="shared" si="1"/>
         <v>94</v>
       </c>
-      <c r="G5" s="29">
+      <c r="H5" s="23">
         <f t="shared" si="2"/>
         <v>64</v>
       </c>
-      <c r="H5" s="29">
+      <c r="I5" s="26">
         <f t="shared" si="3"/>
-        <v>78.333333333333329</v>
-      </c>
-      <c r="I5" s="30">
+        <v>75.5</v>
+      </c>
+      <c r="J5" s="24">
         <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="L5" s="9">
+        <v>45658</v>
+      </c>
+      <c r="N5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="22">
         <v>84</v>
       </c>
-      <c r="C6" s="28">
+      <c r="C6" s="22">
+        <v>84</v>
+      </c>
+      <c r="D6" s="22">
         <v>42</v>
       </c>
-      <c r="D6" s="28">
+      <c r="E6" s="22">
         <v>92</v>
       </c>
-      <c r="E6" s="29">
+      <c r="F6" s="23">
         <f t="shared" si="0"/>
-        <v>218</v>
-      </c>
-      <c r="F6" s="29">
+        <v>302</v>
+      </c>
+      <c r="G6" s="23">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
-      <c r="G6" s="29">
+      <c r="H6" s="23">
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="H6" s="29">
+      <c r="I6" s="26">
         <f t="shared" si="3"/>
-        <v>72.666666666666671</v>
-      </c>
-      <c r="I6" s="30">
+        <v>75.5</v>
+      </c>
+      <c r="J6" s="24">
         <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="9">
+        <v>45658</v>
+      </c>
+      <c r="N6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" s="30" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="32">
+      <c r="B7" s="27">
         <v>43</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="27">
+        <v>29</v>
+      </c>
+      <c r="D7" s="27">
         <v>53</v>
       </c>
-      <c r="D7" s="32">
+      <c r="E7" s="27">
         <v>84</v>
       </c>
-      <c r="E7" s="33">
+      <c r="F7" s="28">
         <f t="shared" si="0"/>
-        <v>180</v>
-      </c>
-      <c r="F7" s="33">
+        <v>209</v>
+      </c>
+      <c r="G7" s="28">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
-      <c r="G7" s="33">
+      <c r="H7" s="28">
         <f t="shared" si="2"/>
-        <v>43</v>
-      </c>
-      <c r="H7" s="33">
+        <v>29</v>
+      </c>
+      <c r="I7" s="29">
         <f t="shared" si="3"/>
-        <v>60</v>
-      </c>
-      <c r="I7" s="34">
+        <v>52.25</v>
+      </c>
+      <c r="J7" s="31">
         <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="L7" s="9">
+        <v>45658</v>
+      </c>
+      <c r="N7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N12" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N13" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>163</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>161</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B16">
         <f>COUNTIF(B2:B7,"&gt;80")</f>
         <v>2</v>
       </c>
-      <c r="C16">
-        <f>MAX(C2:C7)</f>
+      <c r="D16">
+        <f>MAX(D2:D7)</f>
         <v>94</v>
       </c>
-      <c r="D16">
-        <f>AVERAGE(D2:D7)</f>
+      <c r="E16">
+        <f>AVERAGE(E2:E7)</f>
         <v>86.166666666666671</v>
       </c>
     </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>10</v>
+      </c>
+      <c r="B20">
+        <f>$A$20*2</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B21">
+        <f t="shared" ref="B21:B22" si="5">$A$20*2</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B22">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="B2:E7">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>80</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E178CC-A67A-4CEB-9ED6-E0624B3C5E2E}">
-  <dimension ref="A1:AA7"/>
+  <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2333,20 +2811,20 @@
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="2"/>
@@ -2355,76 +2833,76 @@
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
-      <c r="W1" s="17"/>
-      <c r="X1" s="17"/>
-      <c r="Y1" s="17"/>
-      <c r="Z1" s="17"/>
-      <c r="AA1" s="17"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="16" t="s">
+      <c r="C2" s="34"/>
+      <c r="D2" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16" t="s">
+      <c r="C3" s="32"/>
+      <c r="D3" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16" t="s">
+      <c r="C4" s="32"/>
+      <c r="D4" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -2433,19 +2911,19 @@
       <c r="B5" t="s">
         <v>116</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -2454,17 +2932,17 @@
       <c r="B6" t="s">
         <v>116</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -2475,6 +2953,17 @@
       </c>
       <c r="D7" t="s">
         <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B8" t="s">
+        <v>182</v>
+      </c>
+      <c r="D8" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -2494,6 +2983,7 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D3:N3"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2515,26 +3005,26 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="3"/>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21" t="s">
+      <c r="C1" s="36"/>
+      <c r="D1" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="21"/>
+      <c r="E1" s="37"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16" t="s">
+      <c r="C2" s="32"/>
+      <c r="D2" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="16"/>
+      <c r="E2" s="32"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
@@ -2580,10 +3070,10 @@
       <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="16"/>
+      <c r="E8" s="32"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
@@ -2594,99 +3084,99 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="16"/>
+      <c r="C10" s="32"/>
       <c r="D10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16" t="s">
+      <c r="C11" s="32"/>
+      <c r="D11" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="E11" s="16"/>
+      <c r="E11" s="32"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="16" t="s">
+      <c r="C12" s="35"/>
+      <c r="D12" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16" t="s">
+      <c r="C13" s="32"/>
+      <c r="D13" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="E13" s="16"/>
+      <c r="E13" s="32"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>113</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>119</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16" t="s">
+      <c r="C16" s="32"/>
+      <c r="D16" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16" t="s">
+      <c r="C17" s="32"/>
+      <c r="D17" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>130</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
@@ -2709,10 +3199,10 @@
       <c r="B21" t="s">
         <v>137</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="E21" s="16"/>
+      <c r="E21" s="32"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B22" t="s">

</xml_diff>

<commit_message>
Data Entry Completed ( 24-7-2025 )
</commit_message>
<xml_diff>
--- a/Excel/My-Skill-Set-Track.xlsx
+++ b/Excel/My-Skill-Set-Track.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Data-Analytics\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB4BEBC-E965-4A95-A84C-5A4583997337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239DA91F-6EC1-411D-A27B-7B525BE1BC02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{1E7A2102-239A-4535-B10C-B1AF6056B40A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{1E7A2102-239A-4535-B10C-B1AF6056B40A}"/>
   </bookViews>
   <sheets>
     <sheet name="Practice" sheetId="6" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="185">
   <si>
     <t>Topic</t>
   </si>
@@ -594,6 +594,9 @@
   </si>
   <si>
     <t>Solving Problems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total  </t>
   </si>
 </sst>
 </file>
@@ -660,7 +663,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -684,13 +687,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
+      <left style="dotted">
         <color indexed="64"/>
       </left>
       <right style="dotted">
         <color indexed="64"/>
       </right>
-      <top style="thick">
+      <top style="dotted">
         <color indexed="64"/>
       </top>
       <bottom style="dotted">
@@ -702,10 +705,47 @@
       <left style="dotted">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="dotted">
         <color indexed="64"/>
       </right>
-      <top style="thick">
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="dotted">
@@ -717,25 +757,10 @@
       <left style="dotted">
         <color indexed="64"/>
       </left>
-      <right style="thick">
+      <right style="dotted">
         <color indexed="64"/>
       </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dotted">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="dotted">
-        <color indexed="64"/>
-      </right>
-      <top style="dotted">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="dotted">
@@ -747,10 +772,32 @@
       <left style="dotted">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="dotted">
         <color indexed="64"/>
       </right>
-      <top style="dotted">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="dotted">
@@ -762,7 +809,22 @@
       <left style="dotted">
         <color indexed="64"/>
       </left>
-      <right style="thick">
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
         <color indexed="64"/>
       </right>
       <top style="dotted">
@@ -777,17 +839,19 @@
       <left style="dotted">
         <color indexed="64"/>
       </left>
-      <right style="dotted">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="dotted">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="dotted">
@@ -796,20 +860,65 @@
       <top style="dotted">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="dotted">
         <color indexed="64"/>
       </left>
-      <right style="thick">
+      <right style="dotted">
         <color indexed="64"/>
       </right>
       <top style="dotted">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -817,7 +926,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -852,30 +961,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -890,12 +977,332 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="23">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dotted">
+          <color indexed="64"/>
+        </left>
+        <right style="thick">
+          <color indexed="64"/>
+        </right>
+        <top style="dotted">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dotted">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="dotted">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dotted">
+          <color indexed="64"/>
+        </left>
+        <right style="dotted">
+          <color indexed="64"/>
+        </right>
+        <top style="dotted">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dotted">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="dotted">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dotted">
+          <color indexed="64"/>
+        </left>
+        <right style="dotted">
+          <color indexed="64"/>
+        </right>
+        <top style="dotted">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dotted">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="dotted">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dotted">
+          <color indexed="64"/>
+        </left>
+        <right style="dotted">
+          <color indexed="64"/>
+        </right>
+        <top style="dotted">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dotted">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="dotted">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="dotted">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dotted">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="dotted">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dotted">
+          <color indexed="64"/>
+        </left>
+        <right style="dotted">
+          <color indexed="64"/>
+        </right>
+        <top style="dotted">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dotted">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="dotted">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dotted">
+          <color indexed="64"/>
+        </left>
+        <right style="dotted">
+          <color indexed="64"/>
+        </right>
+        <top style="dotted">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dotted">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="dotted">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dotted">
+          <color indexed="64"/>
+        </left>
+        <right style="dotted">
+          <color indexed="64"/>
+        </right>
+        <top style="dotted">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dotted">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="dotted">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dotted">
+          <color indexed="64"/>
+        </left>
+        <right style="dotted">
+          <color indexed="64"/>
+        </right>
+        <top style="dotted">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dotted">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="dotted">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="dotted">
+          <color indexed="64"/>
+        </left>
+        <right style="dotted">
+          <color indexed="64"/>
+        </right>
+        <top style="dotted">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dotted">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="dotted">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color indexed="64"/>
+        </left>
+        <right style="dotted">
+          <color indexed="64"/>
+        </right>
+        <top style="dotted">
+          <color indexed="64"/>
+        </top>
+        <bottom style="dotted">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="dotted">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDF240"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -906,195 +1313,9 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFDDF240"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="dotted">
-          <color indexed="64"/>
-        </left>
-        <right style="thick">
-          <color indexed="64"/>
-        </right>
-        <top style="dotted">
-          <color indexed="64"/>
-        </top>
-        <bottom style="dotted">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="dotted">
-          <color indexed="64"/>
-        </left>
-        <right style="dotted">
-          <color indexed="64"/>
-        </right>
-        <top style="dotted">
-          <color indexed="64"/>
-        </top>
-        <bottom style="dotted">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="dotted">
-          <color indexed="64"/>
-        </left>
-        <right style="dotted">
-          <color indexed="64"/>
-        </right>
-        <top style="dotted">
-          <color indexed="64"/>
-        </top>
-        <bottom style="dotted">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="dotted">
-          <color indexed="64"/>
-        </left>
-        <right style="dotted">
-          <color indexed="64"/>
-        </right>
-        <top style="dotted">
-          <color indexed="64"/>
-        </top>
-        <bottom style="dotted">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="dotted">
-          <color indexed="64"/>
-        </left>
-        <right style="dotted">
-          <color indexed="64"/>
-        </right>
-        <top style="dotted">
-          <color indexed="64"/>
-        </top>
-        <bottom style="dotted">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="dotted">
-          <color indexed="64"/>
-        </left>
-        <right style="dotted">
-          <color indexed="64"/>
-        </right>
-        <top style="dotted">
-          <color indexed="64"/>
-        </top>
-        <bottom style="dotted">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="dotted">
-          <color indexed="64"/>
-        </left>
-        <right style="dotted">
-          <color indexed="64"/>
-        </right>
-        <top style="dotted">
-          <color indexed="64"/>
-        </top>
-        <bottom style="dotted">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="dotted">
-          <color indexed="64"/>
-        </left>
-        <right style="dotted">
-          <color indexed="64"/>
-        </right>
-        <top style="dotted">
-          <color indexed="64"/>
-        </top>
-        <bottom style="dotted">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="dotted">
-          <color indexed="64"/>
-        </left>
-        <right style="dotted">
-          <color indexed="64"/>
-        </right>
-        <top style="dotted">
-          <color indexed="64"/>
-        </top>
-        <bottom style="dotted">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color indexed="64"/>
-        </left>
-        <right style="dotted">
-          <color indexed="64"/>
-        </right>
-        <top style="dotted">
-          <color indexed="64"/>
-        </top>
-        <bottom style="dotted">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1143,8 +1364,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{23555376-2007-4736-A2FA-A02677D80CA8}" name="Table5" displayName="Table5" ref="A1:J7" totalsRowShown="0" headerRowDxfId="13" tableBorderDxfId="12">
-  <autoFilter ref="A1:J7" xr:uid="{23555376-2007-4736-A2FA-A02677D80CA8}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{23555376-2007-4736-A2FA-A02677D80CA8}" name="Table5" displayName="Table5" ref="A1:K7" totalsRowShown="0" headerRowDxfId="22" tableBorderDxfId="21">
+  <autoFilter ref="A1:K7" xr:uid="{23555376-2007-4736-A2FA-A02677D80CA8}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1155,26 +1376,28 @@
     <filterColumn colId="7" hiddenButton="1"/>
     <filterColumn colId="8" hiddenButton="1"/>
     <filterColumn colId="9" hiddenButton="1"/>
+    <filterColumn colId="10" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{DBFED875-5164-47DB-BA0D-B3545E7599AC}" name="Name" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{ED7E621D-B0E7-4E0F-AE49-87626254BEDD}" name="English" dataDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{914CB95C-B4D4-4666-8731-AE771C9B8054}" name="Urdu" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{482F1B75-C013-4781-A7DC-7C06683CBD73}" name="Math" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{A2EB3CEA-91E6-4D55-B25B-F7F6AA16E0F3}" name="Science" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{AF8D4C8A-4FA8-4CD6-AA02-F79836D18D49}" name="SUM" dataDxfId="6">
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{DBFED875-5164-47DB-BA0D-B3545E7599AC}" name="Name" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{ED7E621D-B0E7-4E0F-AE49-87626254BEDD}" name="English" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{914CB95C-B4D4-4666-8731-AE771C9B8054}" name="Urdu" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{482F1B75-C013-4781-A7DC-7C06683CBD73}" name="Math" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{A2EB3CEA-91E6-4D55-B25B-F7F6AA16E0F3}" name="Science" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{AF8D4C8A-4FA8-4CD6-AA02-F79836D18D49}" name="SUM" dataDxfId="11">
       <calculatedColumnFormula>SUM(B2:E2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{7C01B78E-31E9-468C-9645-53B25733C019}" name="MAX" dataDxfId="5">
+    <tableColumn id="11" xr3:uid="{D116192A-F1D0-4240-B555-3C9A2964C5EA}" name="Total  " dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{7C01B78E-31E9-468C-9645-53B25733C019}" name="MAX" dataDxfId="9">
       <calculatedColumnFormula>MAX(B2:E2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3531EF90-C0D8-425F-8DD9-541D509B8B73}" name="MIN" dataDxfId="4">
+    <tableColumn id="7" xr3:uid="{3531EF90-C0D8-425F-8DD9-541D509B8B73}" name="MIN" dataDxfId="8">
       <calculatedColumnFormula>MIN(B2:E2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C539E7AC-D3A5-4230-9E8A-5F7472DD348E}" name="AVG" dataDxfId="3">
+    <tableColumn id="8" xr3:uid="{C539E7AC-D3A5-4230-9E8A-5F7472DD348E}" name="AVG" dataDxfId="7">
       <calculatedColumnFormula>AVERAGE(B2:E2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{CE9690EC-BB92-49C8-A5B5-A7E5A3110BE3}" name="COUNT" dataDxfId="2">
+    <tableColumn id="9" xr3:uid="{CE9690EC-BB92-49C8-A5B5-A7E5A3110BE3}" name="COUNT" dataDxfId="6">
       <calculatedColumnFormula>COUNT(B2:E2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2386,7 +2609,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A2:H22">
-    <cfRule type="expression" dxfId="1" priority="10">
+    <cfRule type="expression" dxfId="17" priority="10">
       <formula>$C2="IT"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2396,21 +2619,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E13B64D4-A1D5-4271-9163-F4CC547F860B}">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="3" width="8.90625" customWidth="1"/>
     <col min="5" max="5" width="9.54296875" customWidth="1"/>
-    <col min="10" max="10" width="8.81640625" customWidth="1"/>
-    <col min="12" max="12" width="11" customWidth="1"/>
+    <col min="11" max="11" width="8.81640625" customWidth="1"/>
+    <col min="13" max="13" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="16" t="s">
         <v>153</v>
       </c>
@@ -2429,311 +2652,332 @@
       <c r="F1" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="H1" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="I1" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="J1" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="K1" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="M1" s="16" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" s="30" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="18">
+      <c r="B2" s="31">
         <v>78</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="31">
         <v>56</v>
       </c>
-      <c r="D2" s="18">
+      <c r="D2" s="31">
         <v>83</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="31">
         <v>91</v>
       </c>
-      <c r="F2" s="19">
+      <c r="F2" s="32">
         <f>SUM(B2:E2)</f>
         <v>308</v>
       </c>
-      <c r="G2" s="19">
+      <c r="G2" s="33">
+        <v>400</v>
+      </c>
+      <c r="H2" s="34">
         <f>MAX(B2:E2)</f>
         <v>91</v>
       </c>
-      <c r="H2" s="19">
+      <c r="I2" s="35">
         <f>MIN(B2:E2)</f>
         <v>56</v>
       </c>
-      <c r="I2" s="25">
+      <c r="J2" s="36">
         <f>AVERAGE(B2:E2)</f>
         <v>77</v>
       </c>
-      <c r="J2" s="20">
+      <c r="K2" s="37">
         <f>COUNT(B2:E2)</f>
         <v>4</v>
       </c>
-      <c r="L2" s="9">
+      <c r="M2" s="9">
         <v>45658</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="21" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" s="38" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="22">
+      <c r="B3" s="17">
         <v>65</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="17">
         <v>74</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="17">
         <v>74</v>
       </c>
-      <c r="E3" s="22">
+      <c r="E3" s="17">
         <v>88</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="26">
         <f t="shared" ref="F3:F7" si="0">SUM(B3:E3)</f>
         <v>301</v>
       </c>
-      <c r="G3" s="23">
-        <f t="shared" ref="G3:G7" si="1">MAX(B3:E3)</f>
+      <c r="G3" s="28">
+        <v>400</v>
+      </c>
+      <c r="H3" s="27">
+        <f t="shared" ref="H3:H7" si="1">MAX(B3:E3)</f>
         <v>88</v>
       </c>
-      <c r="H3" s="23">
-        <f t="shared" ref="H3:H7" si="2">MIN(B3:E3)</f>
+      <c r="I3" s="18">
+        <f t="shared" ref="I3:I7" si="2">MIN(B3:E3)</f>
         <v>65</v>
       </c>
-      <c r="I3" s="26">
-        <f t="shared" ref="I3:I7" si="3">AVERAGE(B3:E3)</f>
+      <c r="J3" s="19">
+        <f t="shared" ref="J3:J7" si="3">AVERAGE(B3:E3)</f>
         <v>75.25</v>
       </c>
-      <c r="J3" s="24">
-        <f t="shared" ref="J3:J7" si="4">COUNT(B3:E3)</f>
+      <c r="K3" s="39">
+        <f t="shared" ref="K3:K7" si="4">COUNT(B3:E3)</f>
         <v>4</v>
       </c>
-      <c r="L3" s="9">
+      <c r="M3" s="9">
         <v>45658</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="21" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B4" s="17">
         <v>90</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="17">
         <v>93</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="17">
         <v>80</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="17">
         <v>85</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="26">
         <f t="shared" si="0"/>
         <v>348</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="28">
+        <v>400</v>
+      </c>
+      <c r="H4" s="27">
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
-      <c r="H4" s="23">
+      <c r="I4" s="18">
         <f t="shared" si="2"/>
         <v>80</v>
       </c>
-      <c r="I4" s="26">
+      <c r="J4" s="19">
         <f t="shared" si="3"/>
         <v>87</v>
       </c>
-      <c r="J4" s="24">
+      <c r="K4" s="39">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="L4" s="9">
+      <c r="M4" s="9">
         <v>45658</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="21" t="s">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" s="38" t="s">
         <v>164</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="17">
         <v>64</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="17">
         <v>67</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="17">
         <v>94</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="17">
         <v>77</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="26">
         <f t="shared" si="0"/>
         <v>302</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="28">
+        <v>400</v>
+      </c>
+      <c r="H5" s="27">
         <f t="shared" si="1"/>
         <v>94</v>
       </c>
-      <c r="H5" s="23">
+      <c r="I5" s="18">
         <f t="shared" si="2"/>
         <v>64</v>
       </c>
-      <c r="I5" s="26">
+      <c r="J5" s="19">
         <f t="shared" si="3"/>
         <v>75.5</v>
       </c>
-      <c r="J5" s="24">
+      <c r="K5" s="39">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="L5" s="9">
+      <c r="M5" s="9">
         <v>45658</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="21" t="s">
+    <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="38" t="s">
         <v>165</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="17">
         <v>84</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="17">
         <v>84</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="17">
         <v>42</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6" s="17">
         <v>92</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="26">
         <f t="shared" si="0"/>
         <v>302</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="28">
+        <v>400</v>
+      </c>
+      <c r="H6" s="27">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
-      <c r="H6" s="23">
+      <c r="I6" s="18">
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="I6" s="26">
+      <c r="J6" s="19">
         <f t="shared" si="3"/>
         <v>75.5</v>
       </c>
-      <c r="J6" s="24">
+      <c r="K6" s="39">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="L6" s="9">
+      <c r="M6" s="9">
         <v>45658</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="30" t="s">
+    <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="40" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="27">
+      <c r="B7" s="41">
         <v>43</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="41">
         <v>29</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="41">
         <v>53</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="41">
         <v>84</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="42">
         <f t="shared" si="0"/>
         <v>209</v>
       </c>
-      <c r="G7" s="28">
+      <c r="G7" s="33">
+        <v>400</v>
+      </c>
+      <c r="H7" s="43">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
-      <c r="H7" s="28">
+      <c r="I7" s="44">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="I7" s="29">
+      <c r="J7" s="45">
         <f t="shared" si="3"/>
         <v>52.25</v>
       </c>
-      <c r="J7" s="31">
+      <c r="K7" s="46">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="L7" s="9">
+      <c r="M7" s="9">
         <v>45658</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="N8" t="s">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="O8" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="N9" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="O9" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="N10" t="s">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="O10" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="N11" t="s">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="O11" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="N12" t="s">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="O12" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="N13" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="O13" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>163</v>
       </c>
@@ -2744,7 +2988,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B16">
         <f>COUNTIF(B2:B7,"&gt;80")</f>
         <v>2</v>
@@ -2782,14 +3026,66 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B2:E7">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
+      <formula>40</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
       <formula>80</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G7">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{E2BB0956-AADD-4B25-9D5F-2C77249C6AB1}</x14:id>
+        </ext>
+      </extLst>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{E2BB0956-AADD-4B25-9D5F-2C77249C6AB1}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G2:G7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="1" id="{A62FFCD7-8667-40D9-9A84-136F4C53B2A4}">
+            <x14:iconSet iconSet="3Stars">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>33</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>67</xm:f>
+              </x14:cfvo>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>E2:E7</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2797,8 +3093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E178CC-A67A-4CEB-9ED6-E0624B3C5E2E}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2811,20 +3107,20 @@
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="2"/>
@@ -2833,76 +3129,76 @@
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33"/>
-      <c r="X1" s="33"/>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="33"/>
-      <c r="AA1" s="33"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="21"/>
+      <c r="V1" s="21"/>
+      <c r="W1" s="21"/>
+      <c r="X1" s="21"/>
+      <c r="Y1" s="21"/>
+      <c r="Z1" s="21"/>
+      <c r="AA1" s="21"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="32" t="s">
+      <c r="C2" s="22"/>
+      <c r="D2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32" t="s">
+      <c r="C3" s="20"/>
+      <c r="D3" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32" t="s">
+      <c r="C4" s="20"/>
+      <c r="D4" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -2911,19 +3207,19 @@
       <c r="B5" t="s">
         <v>116</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -2932,17 +3228,17 @@
       <c r="B6" t="s">
         <v>116</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -2993,7 +3289,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A6F66EB-3F6A-4CB6-B201-8462253FCC87}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -3005,26 +3301,26 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="3"/>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="37" t="s">
+      <c r="C1" s="24"/>
+      <c r="D1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="37"/>
+      <c r="E1" s="25"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="32"/>
+      <c r="E2" s="20"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
@@ -3070,10 +3366,10 @@
       <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="32"/>
+      <c r="E8" s="20"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
@@ -3084,99 +3380,99 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="32"/>
+      <c r="C10" s="20"/>
       <c r="D10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32" t="s">
+      <c r="C11" s="20"/>
+      <c r="D11" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="E11" s="32"/>
+      <c r="E11" s="20"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="C12" s="35"/>
-      <c r="D12" s="32" t="s">
+      <c r="C12" s="23"/>
+      <c r="D12" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32" t="s">
+      <c r="C13" s="20"/>
+      <c r="D13" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="E13" s="32"/>
+      <c r="E13" s="20"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>113</v>
       </c>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>119</v>
       </c>
-      <c r="D15" s="32" t="s">
+      <c r="D15" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32" t="s">
+      <c r="C16" s="20"/>
+      <c r="D16" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32" t="s">
+      <c r="C17" s="20"/>
+      <c r="D17" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>130</v>
       </c>
-      <c r="D18" s="32" t="s">
+      <c r="D18" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
@@ -3199,10 +3495,10 @@
       <c r="B21" t="s">
         <v>137</v>
       </c>
-      <c r="D21" s="32" t="s">
+      <c r="D21" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="E21" s="32"/>
+      <c r="E21" s="20"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B22" t="s">

</xml_diff>

<commit_message>
Learning Data cleaning ( 25-7-2025)
</commit_message>
<xml_diff>
--- a/Excel/My-Skill-Set-Track.xlsx
+++ b/Excel/My-Skill-Set-Track.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Data-Analytics\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239DA91F-6EC1-411D-A27B-7B525BE1BC02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D739EC3-FD45-4E3B-9655-454EB9723BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{1E7A2102-239A-4535-B10C-B1AF6056B40A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Practice" sheetId="6" r:id="rId1"/>
-    <sheet name="Practice Problems" sheetId="8" r:id="rId2"/>
-    <sheet name="Track" sheetId="1" r:id="rId3"/>
-    <sheet name="Shorcut Keys" sheetId="7" r:id="rId4"/>
+    <sheet name="Practice Problems" sheetId="8" r:id="rId1"/>
+    <sheet name="Data Entry" sheetId="6" r:id="rId2"/>
+    <sheet name="Data Cleaning" sheetId="9" r:id="rId3"/>
+    <sheet name="Track" sheetId="1" r:id="rId4"/>
+    <sheet name="Shorcut Keys" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">Track!$A$1:$AA$3</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">Track!$A$1:$AA$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="233">
   <si>
     <t>Topic</t>
   </si>
@@ -597,6 +598,150 @@
   </si>
   <si>
     <t xml:space="preserve">Total  </t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>Frank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  New York  </t>
+  </si>
+  <si>
+    <t>HANNAH</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  hannah  </t>
+  </si>
+  <si>
+    <t>Los Angeles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  eve  </t>
+  </si>
+  <si>
+    <t>chicago</t>
+  </si>
+  <si>
+    <t>miami</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  david  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  charlie  </t>
+  </si>
+  <si>
+    <t>Grace</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>Hannah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ivy  </t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>Eve</t>
+  </si>
+  <si>
+    <t>ALICE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Atlanta  </t>
+  </si>
+  <si>
+    <t>Ivy</t>
+  </si>
+  <si>
+    <t>boston</t>
+  </si>
+  <si>
+    <t>Phoenix</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>phoenix</t>
+  </si>
+  <si>
+    <t>Seattle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  frank  </t>
+  </si>
+  <si>
+    <t>atlanta</t>
+  </si>
+  <si>
+    <t>JACK</t>
+  </si>
+  <si>
+    <t>Denver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Boston  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  grace  </t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
+  <si>
+    <t>denver</t>
+  </si>
+  <si>
+    <t>Atlanta</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  jack  </t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>DAVID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  bob  </t>
+  </si>
+  <si>
+    <t>houston</t>
+  </si>
+  <si>
+    <t>25-7-2025</t>
+  </si>
+  <si>
+    <t>Data Cleaning</t>
   </si>
 </sst>
 </file>
@@ -926,7 +1071,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -963,26 +1108,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1010,12 +1138,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="16">
     <dxf>
       <fill>
         <patternFill>
@@ -1036,34 +1182,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFDDF240"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1288,34 +1407,6 @@
           <color indexed="64"/>
         </horizontal>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDDF240"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1364,7 +1455,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{23555376-2007-4736-A2FA-A02677D80CA8}" name="Table5" displayName="Table5" ref="A1:K7" totalsRowShown="0" headerRowDxfId="22" tableBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{23555376-2007-4736-A2FA-A02677D80CA8}" name="Table5" displayName="Table5" ref="A1:K7" totalsRowShown="0" headerRowDxfId="15" tableBorderDxfId="14">
   <autoFilter ref="A1:K7" xr:uid="{23555376-2007-4736-A2FA-A02677D80CA8}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1379,25 +1470,25 @@
     <filterColumn colId="10" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{DBFED875-5164-47DB-BA0D-B3545E7599AC}" name="Name" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{ED7E621D-B0E7-4E0F-AE49-87626254BEDD}" name="English" dataDxfId="15"/>
-    <tableColumn id="10" xr3:uid="{914CB95C-B4D4-4666-8731-AE771C9B8054}" name="Urdu" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{482F1B75-C013-4781-A7DC-7C06683CBD73}" name="Math" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{A2EB3CEA-91E6-4D55-B25B-F7F6AA16E0F3}" name="Science" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{AF8D4C8A-4FA8-4CD6-AA02-F79836D18D49}" name="SUM" dataDxfId="11">
+    <tableColumn id="1" xr3:uid="{DBFED875-5164-47DB-BA0D-B3545E7599AC}" name="Name" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{ED7E621D-B0E7-4E0F-AE49-87626254BEDD}" name="English" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{914CB95C-B4D4-4666-8731-AE771C9B8054}" name="Urdu" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{482F1B75-C013-4781-A7DC-7C06683CBD73}" name="Math" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{A2EB3CEA-91E6-4D55-B25B-F7F6AA16E0F3}" name="Science" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{AF8D4C8A-4FA8-4CD6-AA02-F79836D18D49}" name="SUM" dataDxfId="8">
       <calculatedColumnFormula>SUM(B2:E2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{D116192A-F1D0-4240-B555-3C9A2964C5EA}" name="Total  " dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{7C01B78E-31E9-468C-9645-53B25733C019}" name="MAX" dataDxfId="9">
+    <tableColumn id="11" xr3:uid="{D116192A-F1D0-4240-B555-3C9A2964C5EA}" name="Total  " dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{7C01B78E-31E9-468C-9645-53B25733C019}" name="MAX" dataDxfId="6">
       <calculatedColumnFormula>MAX(B2:E2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3531EF90-C0D8-425F-8DD9-541D509B8B73}" name="MIN" dataDxfId="8">
+    <tableColumn id="7" xr3:uid="{3531EF90-C0D8-425F-8DD9-541D509B8B73}" name="MIN" dataDxfId="5">
       <calculatedColumnFormula>MIN(B2:E2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C539E7AC-D3A5-4230-9E8A-5F7472DD348E}" name="AVG" dataDxfId="7">
+    <tableColumn id="8" xr3:uid="{C539E7AC-D3A5-4230-9E8A-5F7472DD348E}" name="AVG" dataDxfId="4">
       <calculatedColumnFormula>AVERAGE(B2:E2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{CE9690EC-BB92-49C8-A5B5-A7E5A3110BE3}" name="COUNT" dataDxfId="6">
+    <tableColumn id="9" xr3:uid="{CE9690EC-BB92-49C8-A5B5-A7E5A3110BE3}" name="COUNT" dataDxfId="3">
       <calculatedColumnFormula>COUNT(B2:E2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1721,907 +1812,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E0F8151-937B-4935-B8F3-24E8BCB42125}">
-  <dimension ref="A1:S23"/>
-  <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="9.36328125" customWidth="1"/>
-    <col min="2" max="2" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" customWidth="1"/>
-    <col min="4" max="4" width="12.1796875" style="14" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="5.36328125" customWidth="1"/>
-    <col min="7" max="7" width="16.36328125" customWidth="1"/>
-    <col min="8" max="8" width="14.7265625" style="9" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D2" s="13">
-        <v>38000</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" s="6">
-        <v>20</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="H2" s="11">
-        <v>45661</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D3" s="13">
-        <v>36000</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" s="6">
-        <v>21</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="H3" s="11">
-        <v>45662</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="D4" s="13">
-        <v>34000</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" s="6">
-        <v>21</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="H4" s="11">
-        <v>45663</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D5" s="13">
-        <v>32000</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="6">
-        <v>20</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="H5" s="11">
-        <v>45664</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D6" s="13">
-        <v>30000</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" s="6">
-        <v>23</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="H6" s="11">
-        <v>45665</v>
-      </c>
-      <c r="L6" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="M6" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="N6" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="O6" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="P6" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q6" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="R6" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="S6" s="15" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="D7" s="13">
-        <v>28000</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F7" s="6">
-        <v>24</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="H7" s="11">
-        <v>45666</v>
-      </c>
-      <c r="L7">
-        <v>85</v>
-      </c>
-      <c r="M7">
-        <v>37</v>
-      </c>
-      <c r="N7">
-        <v>25</v>
-      </c>
-      <c r="O7">
-        <f>SUM(L7:N7)+$L$19</f>
-        <v>157</v>
-      </c>
-      <c r="P7">
-        <f>MAX(L7:N7)</f>
-        <v>85</v>
-      </c>
-      <c r="Q7">
-        <f>MIN(L7:N7)</f>
-        <v>25</v>
-      </c>
-      <c r="R7">
-        <f>AVERAGE(L7:N7)</f>
-        <v>49</v>
-      </c>
-      <c r="S7">
-        <f>COUNT(L7:N7)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="D8" s="13">
-        <v>26000</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="6">
-        <v>23</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="H8" s="11">
-        <v>45667</v>
-      </c>
-      <c r="L8">
-        <v>48</v>
-      </c>
-      <c r="M8">
-        <v>18</v>
-      </c>
-      <c r="N8">
-        <v>48</v>
-      </c>
-      <c r="O8">
-        <f t="shared" ref="O8:O16" si="0">SUM(L8:N8)+$L$19</f>
-        <v>124</v>
-      </c>
-      <c r="P8">
-        <f t="shared" ref="P8:P16" si="1">MAX(L8:N8)</f>
-        <v>48</v>
-      </c>
-      <c r="Q8">
-        <f t="shared" ref="Q8:Q16" si="2">MIN(L8:N8)</f>
-        <v>18</v>
-      </c>
-      <c r="R8">
-        <f t="shared" ref="R8:R16" si="3">AVERAGE(L8:N8)</f>
-        <v>38</v>
-      </c>
-      <c r="S8">
-        <f t="shared" ref="S8:S15" si="4">COUNT(L8:N8)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D9" s="13">
-        <v>24000</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="6">
-        <v>26</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="H9" s="11">
-        <v>45668</v>
-      </c>
-      <c r="L9">
-        <v>39</v>
-      </c>
-      <c r="M9">
-        <v>72</v>
-      </c>
-      <c r="N9">
-        <v>58</v>
-      </c>
-      <c r="O9">
-        <f t="shared" si="0"/>
-        <v>179</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="1"/>
-        <v>72</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="2"/>
-        <v>39</v>
-      </c>
-      <c r="R9">
-        <f t="shared" si="3"/>
-        <v>56.333333333333336</v>
-      </c>
-      <c r="S9">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D10" s="13">
-        <v>22000</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" s="6">
-        <v>28</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="H10" s="11">
-        <v>45669</v>
-      </c>
-      <c r="L10">
-        <v>29</v>
-      </c>
-      <c r="M10">
-        <v>40</v>
-      </c>
-      <c r="N10">
-        <v>49</v>
-      </c>
-      <c r="O10">
-        <f t="shared" si="0"/>
-        <v>128</v>
-      </c>
-      <c r="P10">
-        <f t="shared" si="1"/>
-        <v>49</v>
-      </c>
-      <c r="Q10">
-        <f t="shared" si="2"/>
-        <v>29</v>
-      </c>
-      <c r="R10">
-        <f t="shared" si="3"/>
-        <v>39.333333333333336</v>
-      </c>
-      <c r="S10">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D11" s="13">
-        <v>20000</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11" s="6">
-        <v>30</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="H11" s="11">
-        <v>45670</v>
-      </c>
-      <c r="L11">
-        <v>74</v>
-      </c>
-      <c r="M11">
-        <v>99</v>
-      </c>
-      <c r="N11">
-        <v>70</v>
-      </c>
-      <c r="O11">
-        <f t="shared" si="0"/>
-        <v>253</v>
-      </c>
-      <c r="P11">
-        <f t="shared" si="1"/>
-        <v>99</v>
-      </c>
-      <c r="Q11">
-        <f t="shared" si="2"/>
-        <v>70</v>
-      </c>
-      <c r="R11">
-        <f t="shared" si="3"/>
-        <v>81</v>
-      </c>
-      <c r="S11">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D12" s="13">
-        <v>18000</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="6">
-        <v>20</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="H12" s="11">
-        <v>45671</v>
-      </c>
-      <c r="L12">
-        <v>32</v>
-      </c>
-      <c r="M12">
-        <v>81</v>
-      </c>
-      <c r="N12">
-        <v>26</v>
-      </c>
-      <c r="O12">
-        <f t="shared" si="0"/>
-        <v>149</v>
-      </c>
-      <c r="P12">
-        <f t="shared" si="1"/>
-        <v>81</v>
-      </c>
-      <c r="Q12">
-        <f t="shared" si="2"/>
-        <v>26</v>
-      </c>
-      <c r="R12">
-        <f t="shared" si="3"/>
-        <v>46.333333333333336</v>
-      </c>
-      <c r="S12">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D13" s="13">
-        <v>16000</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="6">
-        <v>23</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="H13" s="11">
-        <v>45672</v>
-      </c>
-      <c r="L13">
-        <v>49</v>
-      </c>
-      <c r="M13">
-        <v>47</v>
-      </c>
-      <c r="N13">
-        <v>94</v>
-      </c>
-      <c r="O13">
-        <f t="shared" si="0"/>
-        <v>200</v>
-      </c>
-      <c r="P13">
-        <f t="shared" si="1"/>
-        <v>94</v>
-      </c>
-      <c r="Q13">
-        <f t="shared" si="2"/>
-        <v>47</v>
-      </c>
-      <c r="R13">
-        <f t="shared" si="3"/>
-        <v>63.333333333333336</v>
-      </c>
-      <c r="S13">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="D14" s="13">
-        <v>14000</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F14" s="6">
-        <v>21</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="H14" s="11">
-        <v>45673</v>
-      </c>
-      <c r="L14">
-        <v>46</v>
-      </c>
-      <c r="M14">
-        <v>29</v>
-      </c>
-      <c r="N14">
-        <v>93</v>
-      </c>
-      <c r="O14">
-        <f t="shared" si="0"/>
-        <v>178</v>
-      </c>
-      <c r="P14">
-        <f t="shared" si="1"/>
-        <v>93</v>
-      </c>
-      <c r="Q14">
-        <f t="shared" si="2"/>
-        <v>29</v>
-      </c>
-      <c r="R14">
-        <f t="shared" si="3"/>
-        <v>56</v>
-      </c>
-      <c r="S14">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="D15" s="13">
-        <v>12000</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F15" s="6">
-        <v>25</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="H15" s="11">
-        <v>45674</v>
-      </c>
-      <c r="L15">
-        <v>94</v>
-      </c>
-      <c r="M15">
-        <v>4</v>
-      </c>
-      <c r="N15">
-        <v>51</v>
-      </c>
-      <c r="O15">
-        <f t="shared" si="0"/>
-        <v>159</v>
-      </c>
-      <c r="P15">
-        <f t="shared" si="1"/>
-        <v>94</v>
-      </c>
-      <c r="Q15">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="R15">
-        <f t="shared" si="3"/>
-        <v>49.666666666666664</v>
-      </c>
-      <c r="S15">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D16" s="13">
-        <v>10000</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F16" s="6">
-        <v>25</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="H16" s="11">
-        <v>45675</v>
-      </c>
-      <c r="L16">
-        <v>52</v>
-      </c>
-      <c r="M16">
-        <v>75</v>
-      </c>
-      <c r="N16">
-        <v>31</v>
-      </c>
-      <c r="O16">
-        <f t="shared" si="0"/>
-        <v>168</v>
-      </c>
-      <c r="P16">
-        <f t="shared" si="1"/>
-        <v>75</v>
-      </c>
-      <c r="Q16">
-        <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
-      <c r="R16">
-        <f t="shared" si="3"/>
-        <v>52.666666666666664</v>
-      </c>
-      <c r="S16">
-        <f>COUNT(L16:N16)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A17" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="D17" s="13">
-        <v>8000</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F17" s="6">
-        <v>21</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="H17" s="11">
-        <v>45676</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A18" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="D18" s="13">
-        <v>6000</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F18" s="6">
-        <v>20</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="H18" s="11">
-        <v>45677</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A19" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D19" s="13">
-        <v>4000</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F19" s="6">
-        <v>20</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="H19" s="11">
-        <v>45678</v>
-      </c>
-      <c r="L19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A20" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D20" s="13">
-        <v>2000</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="F20" s="6">
-        <v>20</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="H20" s="11">
-        <v>45679</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A21" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D21" s="13">
-        <v>2000</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F21" s="6">
-        <v>28</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="C23" s="4"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A2:H22">
-    <cfRule type="expression" dxfId="17" priority="10">
-      <formula>$C2="IT"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E13B64D4-A1D5-4271-9163-F4CC547F860B}">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -2652,7 +1846,7 @@
       <c r="F1" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="16" t="s">
         <v>184</v>
       </c>
       <c r="H1" s="16" t="s">
@@ -2672,41 +1866,41 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="23" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="31">
+      <c r="B2" s="24">
         <v>78</v>
       </c>
-      <c r="C2" s="31">
+      <c r="C2" s="24">
         <v>56</v>
       </c>
-      <c r="D2" s="31">
+      <c r="D2" s="24">
         <v>83</v>
       </c>
-      <c r="E2" s="31">
+      <c r="E2" s="24">
         <v>91</v>
       </c>
-      <c r="F2" s="32">
+      <c r="F2" s="25">
         <f>SUM(B2:E2)</f>
         <v>308</v>
       </c>
-      <c r="G2" s="33">
+      <c r="G2" s="26">
         <v>400</v>
       </c>
-      <c r="H2" s="34">
+      <c r="H2" s="27">
         <f>MAX(B2:E2)</f>
         <v>91</v>
       </c>
-      <c r="I2" s="35">
+      <c r="I2" s="28">
         <f>MIN(B2:E2)</f>
         <v>56</v>
       </c>
-      <c r="J2" s="36">
+      <c r="J2" s="29">
         <f>AVERAGE(B2:E2)</f>
         <v>77</v>
       </c>
-      <c r="K2" s="37">
+      <c r="K2" s="30">
         <f>COUNT(B2:E2)</f>
         <v>4</v>
       </c>
@@ -2718,7 +1912,7 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="31" t="s">
         <v>158</v>
       </c>
       <c r="B3" s="17">
@@ -2733,14 +1927,14 @@
       <c r="E3" s="17">
         <v>88</v>
       </c>
-      <c r="F3" s="26">
+      <c r="F3" s="20">
         <f t="shared" ref="F3:F7" si="0">SUM(B3:E3)</f>
         <v>301</v>
       </c>
-      <c r="G3" s="28">
+      <c r="G3" s="22">
         <v>400</v>
       </c>
-      <c r="H3" s="27">
+      <c r="H3" s="21">
         <f t="shared" ref="H3:H7" si="1">MAX(B3:E3)</f>
         <v>88</v>
       </c>
@@ -2752,7 +1946,7 @@
         <f t="shared" ref="J3:J7" si="3">AVERAGE(B3:E3)</f>
         <v>75.25</v>
       </c>
-      <c r="K3" s="39">
+      <c r="K3" s="32">
         <f t="shared" ref="K3:K7" si="4">COUNT(B3:E3)</f>
         <v>4</v>
       </c>
@@ -2764,7 +1958,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="31" t="s">
         <v>159</v>
       </c>
       <c r="B4" s="17">
@@ -2779,14 +1973,14 @@
       <c r="E4" s="17">
         <v>85</v>
       </c>
-      <c r="F4" s="26">
+      <c r="F4" s="20">
         <f t="shared" si="0"/>
         <v>348</v>
       </c>
-      <c r="G4" s="28">
+      <c r="G4" s="22">
         <v>400</v>
       </c>
-      <c r="H4" s="27">
+      <c r="H4" s="21">
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
@@ -2798,7 +1992,7 @@
         <f t="shared" si="3"/>
         <v>87</v>
       </c>
-      <c r="K4" s="39">
+      <c r="K4" s="32">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
@@ -2810,7 +2004,7 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="31" t="s">
         <v>164</v>
       </c>
       <c r="B5" s="17">
@@ -2825,14 +2019,14 @@
       <c r="E5" s="17">
         <v>77</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="20">
         <f t="shared" si="0"/>
         <v>302</v>
       </c>
-      <c r="G5" s="28">
+      <c r="G5" s="22">
         <v>400</v>
       </c>
-      <c r="H5" s="27">
+      <c r="H5" s="21">
         <f t="shared" si="1"/>
         <v>94</v>
       </c>
@@ -2844,7 +2038,7 @@
         <f t="shared" si="3"/>
         <v>75.5</v>
       </c>
-      <c r="K5" s="39">
+      <c r="K5" s="32">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
@@ -2856,7 +2050,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="31" t="s">
         <v>165</v>
       </c>
       <c r="B6" s="17">
@@ -2871,14 +2065,14 @@
       <c r="E6" s="17">
         <v>92</v>
       </c>
-      <c r="F6" s="26">
+      <c r="F6" s="20">
         <f t="shared" si="0"/>
         <v>302</v>
       </c>
-      <c r="G6" s="28">
+      <c r="G6" s="22">
         <v>400</v>
       </c>
-      <c r="H6" s="27">
+      <c r="H6" s="21">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
@@ -2890,7 +2084,7 @@
         <f t="shared" si="3"/>
         <v>75.5</v>
       </c>
-      <c r="K6" s="39">
+      <c r="K6" s="32">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
@@ -2902,41 +2096,41 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="33" t="s">
         <v>166</v>
       </c>
-      <c r="B7" s="41">
+      <c r="B7" s="34">
         <v>43</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C7" s="34">
         <v>29</v>
       </c>
-      <c r="D7" s="41">
+      <c r="D7" s="34">
         <v>53</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="34">
         <v>84</v>
       </c>
-      <c r="F7" s="42">
+      <c r="F7" s="35">
         <f t="shared" si="0"/>
         <v>209</v>
       </c>
-      <c r="G7" s="33">
+      <c r="G7" s="26">
         <v>400</v>
       </c>
-      <c r="H7" s="43">
+      <c r="H7" s="36">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
-      <c r="I7" s="44">
+      <c r="I7" s="37">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="J7" s="45">
+      <c r="J7" s="38">
         <f t="shared" si="3"/>
         <v>52.25</v>
       </c>
-      <c r="K7" s="46">
+      <c r="K7" s="39">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
@@ -3026,10 +2220,10 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B2:E7">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="lessThan">
       <formula>40</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThan">
       <formula>80</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3055,19 +2249,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{E2BB0956-AADD-4B25-9D5F-2C77249C6AB1}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FF638EC6"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>G2:G7</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="1" id="{A62FFCD7-8667-40D9-9A84-136F4C53B2A4}">
             <x14:iconSet iconSet="3Stars">
               <x14:cfvo type="percent">
@@ -3083,15 +2264,1599 @@
           </x14:cfRule>
           <xm:sqref>E2:E7</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{E2BB0956-AADD-4B25-9D5F-2C77249C6AB1}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G2:G7</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E0F8151-937B-4935-B8F3-24E8BCB42125}">
+  <dimension ref="A1:S23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.36328125" customWidth="1"/>
+    <col min="2" max="2" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" style="14" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="5.36328125" customWidth="1"/>
+    <col min="7" max="7" width="16.36328125" customWidth="1"/>
+    <col min="8" max="8" width="14.7265625" style="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="13">
+        <v>38000</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="6">
+        <v>20</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H2" s="11">
+        <v>45661</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="13">
+        <v>36000</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="6">
+        <v>21</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H3" s="11">
+        <v>45662</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="13">
+        <v>34000</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="6">
+        <v>21</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="11">
+        <v>45663</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="13">
+        <v>32000</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="6">
+        <v>20</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="H5" s="11">
+        <v>45664</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="13">
+        <v>30000</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="6">
+        <v>23</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="H6" s="11">
+        <v>45665</v>
+      </c>
+      <c r="L6" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="M6" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="N6" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="O6" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="P6" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q6" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="R6" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="S6" s="15" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="13">
+        <v>28000</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="6">
+        <v>24</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="H7" s="11">
+        <v>45666</v>
+      </c>
+      <c r="L7">
+        <v>85</v>
+      </c>
+      <c r="M7">
+        <v>37</v>
+      </c>
+      <c r="N7">
+        <v>25</v>
+      </c>
+      <c r="O7">
+        <f>SUM(L7:N7)+$L$19</f>
+        <v>157</v>
+      </c>
+      <c r="P7">
+        <f>MAX(L7:N7)</f>
+        <v>85</v>
+      </c>
+      <c r="Q7">
+        <f>MIN(L7:N7)</f>
+        <v>25</v>
+      </c>
+      <c r="R7">
+        <f>AVERAGE(L7:N7)</f>
+        <v>49</v>
+      </c>
+      <c r="S7">
+        <f>COUNT(L7:N7)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="13">
+        <v>26000</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="6">
+        <v>23</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="H8" s="11">
+        <v>45667</v>
+      </c>
+      <c r="L8">
+        <v>48</v>
+      </c>
+      <c r="M8">
+        <v>18</v>
+      </c>
+      <c r="N8">
+        <v>48</v>
+      </c>
+      <c r="O8">
+        <f t="shared" ref="O8:O16" si="0">SUM(L8:N8)+$L$19</f>
+        <v>124</v>
+      </c>
+      <c r="P8">
+        <f t="shared" ref="P8:P16" si="1">MAX(L8:N8)</f>
+        <v>48</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" ref="Q8:Q16" si="2">MIN(L8:N8)</f>
+        <v>18</v>
+      </c>
+      <c r="R8">
+        <f t="shared" ref="R8:R16" si="3">AVERAGE(L8:N8)</f>
+        <v>38</v>
+      </c>
+      <c r="S8">
+        <f t="shared" ref="S8:S15" si="4">COUNT(L8:N8)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="13">
+        <v>24000</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="6">
+        <v>26</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" s="11">
+        <v>45668</v>
+      </c>
+      <c r="L9">
+        <v>39</v>
+      </c>
+      <c r="M9">
+        <v>72</v>
+      </c>
+      <c r="N9">
+        <v>58</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>179</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="3"/>
+        <v>56.333333333333336</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" s="13">
+        <v>22000</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="6">
+        <v>28</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H10" s="11">
+        <v>45669</v>
+      </c>
+      <c r="L10">
+        <v>29</v>
+      </c>
+      <c r="M10">
+        <v>40</v>
+      </c>
+      <c r="N10">
+        <v>49</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="3"/>
+        <v>39.333333333333336</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" s="13">
+        <v>20000</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="6">
+        <v>30</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="H11" s="11">
+        <v>45670</v>
+      </c>
+      <c r="L11">
+        <v>74</v>
+      </c>
+      <c r="M11">
+        <v>99</v>
+      </c>
+      <c r="N11">
+        <v>70</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>253</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="3"/>
+        <v>81</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" s="13">
+        <v>18000</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="6">
+        <v>20</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="H12" s="11">
+        <v>45671</v>
+      </c>
+      <c r="L12">
+        <v>32</v>
+      </c>
+      <c r="M12">
+        <v>81</v>
+      </c>
+      <c r="N12">
+        <v>26</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>149</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="3"/>
+        <v>46.333333333333336</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" s="13">
+        <v>16000</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="6">
+        <v>23</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="H13" s="11">
+        <v>45672</v>
+      </c>
+      <c r="L13">
+        <v>49</v>
+      </c>
+      <c r="M13">
+        <v>47</v>
+      </c>
+      <c r="N13">
+        <v>94</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="3"/>
+        <v>63.333333333333336</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="13">
+        <v>14000</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" s="6">
+        <v>21</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="H14" s="11">
+        <v>45673</v>
+      </c>
+      <c r="L14">
+        <v>46</v>
+      </c>
+      <c r="M14">
+        <v>29</v>
+      </c>
+      <c r="N14">
+        <v>93</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="0"/>
+        <v>178</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="3"/>
+        <v>56</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" s="13">
+        <v>12000</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" s="6">
+        <v>25</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="H15" s="11">
+        <v>45674</v>
+      </c>
+      <c r="L15">
+        <v>94</v>
+      </c>
+      <c r="M15">
+        <v>4</v>
+      </c>
+      <c r="N15">
+        <v>51</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="0"/>
+        <v>159</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="3"/>
+        <v>49.666666666666664</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="13">
+        <v>10000</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" s="6">
+        <v>25</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H16" s="11">
+        <v>45675</v>
+      </c>
+      <c r="L16">
+        <v>52</v>
+      </c>
+      <c r="M16">
+        <v>75</v>
+      </c>
+      <c r="N16">
+        <v>31</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="0"/>
+        <v>168</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="3"/>
+        <v>52.666666666666664</v>
+      </c>
+      <c r="S16">
+        <f>COUNT(L16:N16)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D17" s="13">
+        <v>8000</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F17" s="6">
+        <v>21</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="H17" s="11">
+        <v>45676</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" s="13">
+        <v>6000</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="6">
+        <v>20</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="H18" s="11">
+        <v>45677</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="13">
+        <v>4000</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="6">
+        <v>20</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="H19" s="11">
+        <v>45678</v>
+      </c>
+      <c r="L19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20" s="13">
+        <v>2000</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" s="6">
+        <v>20</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H20" s="11">
+        <v>45679</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21" s="13">
+        <v>2000</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F21" s="6">
+        <v>28</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C23" s="4"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="A2:H22">
+    <cfRule type="expression" dxfId="2" priority="10">
+      <formula>$C2="IT"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79D2C3E0-16F0-44E3-9BCD-828BC7817756}">
+  <dimension ref="A1:D58"/>
+  <sheetViews>
+    <sheetView zoomScale="103" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="47" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="47" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" s="47" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46" t="s">
+        <v>188</v>
+      </c>
+      <c r="D2" s="46">
+        <v>60960</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="46" t="s">
+        <v>189</v>
+      </c>
+      <c r="B3" s="46">
+        <v>-4</v>
+      </c>
+      <c r="C3" s="46" t="s">
+        <v>190</v>
+      </c>
+      <c r="D3" s="46">
+        <v>-8832</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="46" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46" t="s">
+        <v>192</v>
+      </c>
+      <c r="D4" s="46">
+        <v>70288</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="46" t="s">
+        <v>193</v>
+      </c>
+      <c r="B5" s="46">
+        <v>-15</v>
+      </c>
+      <c r="C5" s="46" t="s">
+        <v>194</v>
+      </c>
+      <c r="D5" s="46">
+        <v>-14166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="B6" s="46">
+        <v>46</v>
+      </c>
+      <c r="C6" s="46" t="s">
+        <v>196</v>
+      </c>
+      <c r="D6" s="46">
+        <v>34721</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="46" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="46" t="s">
+        <v>193</v>
+      </c>
+      <c r="B8" s="46">
+        <v>22</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>197</v>
+      </c>
+      <c r="D8" s="46">
+        <v>-7809</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="46"/>
+      <c r="B9" s="46">
+        <v>-18</v>
+      </c>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46">
+        <v>88176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="46" t="s">
+        <v>199</v>
+      </c>
+      <c r="B10" s="46">
+        <v>-4</v>
+      </c>
+      <c r="C10" s="46" t="s">
+        <v>188</v>
+      </c>
+      <c r="D10" s="46">
+        <v>86833</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="46" t="s">
+        <v>200</v>
+      </c>
+      <c r="B11" s="46"/>
+      <c r="C11" s="46" t="s">
+        <v>201</v>
+      </c>
+      <c r="D11" s="46">
+        <v>-31634</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="46" t="s">
+        <v>202</v>
+      </c>
+      <c r="B12" s="46">
+        <v>-3</v>
+      </c>
+      <c r="C12" s="46" t="s">
+        <v>201</v>
+      </c>
+      <c r="D12" s="46">
+        <v>-7552</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="46" t="s">
+        <v>203</v>
+      </c>
+      <c r="B13" s="46"/>
+      <c r="C13" s="46" t="s">
+        <v>201</v>
+      </c>
+      <c r="D13" s="46">
+        <v>-49232</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="46" t="s">
+        <v>204</v>
+      </c>
+      <c r="B14" s="46">
+        <v>-16</v>
+      </c>
+      <c r="C14" s="46" t="s">
+        <v>205</v>
+      </c>
+      <c r="D14" s="46">
+        <v>-48628</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="46" t="s">
+        <v>206</v>
+      </c>
+      <c r="B15" s="46">
+        <v>46</v>
+      </c>
+      <c r="C15" s="46" t="s">
+        <v>188</v>
+      </c>
+      <c r="D15" s="46">
+        <v>-48261</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="46" t="s">
+        <v>207</v>
+      </c>
+      <c r="B16" s="46">
+        <v>28</v>
+      </c>
+      <c r="C16" s="46" t="s">
+        <v>208</v>
+      </c>
+      <c r="D16" s="46">
+        <v>-28901</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="46" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="18" spans="1:4" s="46" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="46" t="s">
+        <v>209</v>
+      </c>
+      <c r="B19" s="46"/>
+      <c r="C19" s="46" t="s">
+        <v>210</v>
+      </c>
+      <c r="D19" s="46">
+        <v>63512</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="46" t="s">
+        <v>206</v>
+      </c>
+      <c r="B20" s="46">
+        <v>-5</v>
+      </c>
+      <c r="C20" s="46" t="s">
+        <v>211</v>
+      </c>
+      <c r="D20" s="46">
+        <v>-7670</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="46" t="s">
+        <v>212</v>
+      </c>
+      <c r="B21" s="46">
+        <v>-6</v>
+      </c>
+      <c r="C21" s="46" t="s">
+        <v>213</v>
+      </c>
+      <c r="D21" s="46">
+        <v>-30278</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="46" t="s">
+        <v>202</v>
+      </c>
+      <c r="B22" s="46">
+        <v>-12</v>
+      </c>
+      <c r="C22" s="46"/>
+      <c r="D22" s="46">
+        <v>-44867</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="46" t="s">
+        <v>212</v>
+      </c>
+      <c r="B23" s="46"/>
+      <c r="C23" s="46" t="s">
+        <v>214</v>
+      </c>
+      <c r="D23" s="46">
+        <v>55450</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="B24" s="46">
+        <v>-1</v>
+      </c>
+      <c r="C24" s="46" t="s">
+        <v>214</v>
+      </c>
+      <c r="D24" s="46">
+        <v>61024</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="46" t="s">
+        <v>189</v>
+      </c>
+      <c r="B25" s="46">
+        <v>-2</v>
+      </c>
+      <c r="C25" s="46" t="s">
+        <v>194</v>
+      </c>
+      <c r="D25" s="46">
+        <v>-20466</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="46" t="s">
+        <v>215</v>
+      </c>
+      <c r="B26" s="46">
+        <v>32</v>
+      </c>
+      <c r="C26" s="46" t="s">
+        <v>201</v>
+      </c>
+      <c r="D26" s="46">
+        <v>68810</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="46" t="s">
+        <v>193</v>
+      </c>
+      <c r="B27" s="46">
+        <v>-10</v>
+      </c>
+      <c r="C27" s="46" t="s">
+        <v>188</v>
+      </c>
+      <c r="D27" s="46">
+        <v>52418</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="46" t="s">
+        <v>199</v>
+      </c>
+      <c r="B28" s="46">
+        <v>30</v>
+      </c>
+      <c r="C28" s="46" t="s">
+        <v>216</v>
+      </c>
+      <c r="D28" s="46">
+        <v>-24695</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="46" t="s">
+        <v>215</v>
+      </c>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46" t="s">
+        <v>197</v>
+      </c>
+      <c r="D29" s="46">
+        <v>66768</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="46" t="s">
+        <v>207</v>
+      </c>
+      <c r="B30" s="46">
+        <v>46</v>
+      </c>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46">
+        <v>47903</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="46" t="s">
+        <v>217</v>
+      </c>
+      <c r="B31" s="46"/>
+      <c r="C31" s="46" t="s">
+        <v>218</v>
+      </c>
+      <c r="D31" s="46">
+        <v>57073</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" s="46" t="s">
+        <v>204</v>
+      </c>
+      <c r="B32" s="46"/>
+      <c r="C32" s="46" t="s">
+        <v>219</v>
+      </c>
+      <c r="D32" s="46">
+        <v>67004</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="46" t="s">
+        <v>220</v>
+      </c>
+      <c r="B33" s="46">
+        <v>34</v>
+      </c>
+      <c r="C33" s="46" t="s">
+        <v>213</v>
+      </c>
+      <c r="D33" s="46">
+        <v>80313</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="46" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="35" spans="1:4" s="46" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="46" t="s">
+        <v>203</v>
+      </c>
+      <c r="B36" s="46">
+        <v>-18</v>
+      </c>
+      <c r="C36" s="46" t="s">
+        <v>201</v>
+      </c>
+      <c r="D36" s="46">
+        <v>-29609</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="46" t="s">
+        <v>221</v>
+      </c>
+      <c r="B37" s="46">
+        <v>-17</v>
+      </c>
+      <c r="C37" s="46"/>
+      <c r="D37" s="46">
+        <v>-37817</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" s="46" t="s">
+        <v>206</v>
+      </c>
+      <c r="B38" s="46"/>
+      <c r="C38" s="46" t="s">
+        <v>222</v>
+      </c>
+      <c r="D38" s="46">
+        <v>-19447</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="46" t="s">
+        <v>198</v>
+      </c>
+      <c r="B39" s="46"/>
+      <c r="C39" s="46" t="s">
+        <v>223</v>
+      </c>
+      <c r="D39" s="46">
+        <v>63644</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" s="46" t="s">
+        <v>204</v>
+      </c>
+      <c r="B40" s="46"/>
+      <c r="C40" s="46" t="s">
+        <v>223</v>
+      </c>
+      <c r="D40" s="46">
+        <v>38532</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" s="46" t="s">
+        <v>189</v>
+      </c>
+      <c r="B41" s="46"/>
+      <c r="C41" s="46"/>
+      <c r="D41" s="46">
+        <v>73530</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" s="46" t="s">
+        <v>189</v>
+      </c>
+      <c r="B42" s="46"/>
+      <c r="C42" s="46" t="s">
+        <v>205</v>
+      </c>
+      <c r="D42" s="46">
+        <v>-23100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" s="46" t="s">
+        <v>221</v>
+      </c>
+      <c r="B43" s="46">
+        <v>27</v>
+      </c>
+      <c r="C43" s="46" t="s">
+        <v>224</v>
+      </c>
+      <c r="D43" s="46">
+        <v>-37762</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" s="46" t="s">
+        <v>225</v>
+      </c>
+      <c r="B44" s="46"/>
+      <c r="C44" s="46"/>
+      <c r="D44" s="46">
+        <v>-17736</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="46" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" s="46" t="s">
+        <v>212</v>
+      </c>
+      <c r="B46" s="46"/>
+      <c r="C46" s="46" t="s">
+        <v>197</v>
+      </c>
+      <c r="D46" s="46">
+        <v>56244</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" s="46" t="s">
+        <v>203</v>
+      </c>
+      <c r="B47" s="46">
+        <v>30</v>
+      </c>
+      <c r="C47" s="46" t="s">
+        <v>190</v>
+      </c>
+      <c r="D47" s="46">
+        <v>-47178</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="B48" s="46">
+        <v>-18</v>
+      </c>
+      <c r="C48" s="46" t="s">
+        <v>201</v>
+      </c>
+      <c r="D48" s="46">
+        <v>33630</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" s="46" t="s">
+        <v>221</v>
+      </c>
+      <c r="B49" s="46"/>
+      <c r="C49" s="46" t="s">
+        <v>216</v>
+      </c>
+      <c r="D49" s="46">
+        <v>64648</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50" s="46" t="s">
+        <v>227</v>
+      </c>
+      <c r="B50" s="46"/>
+      <c r="C50" s="46" t="s">
+        <v>211</v>
+      </c>
+      <c r="D50" s="46">
+        <v>-11482</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51" s="46" t="s">
+        <v>228</v>
+      </c>
+      <c r="B51" s="46"/>
+      <c r="C51" s="46" t="s">
+        <v>224</v>
+      </c>
+      <c r="D51" s="46">
+        <v>-31280</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" s="46" t="s">
+        <v>202</v>
+      </c>
+      <c r="B52" s="46">
+        <v>49</v>
+      </c>
+      <c r="C52" s="46" t="s">
+        <v>210</v>
+      </c>
+      <c r="D52" s="46">
+        <v>86721</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" s="46" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" s="46" t="s">
+        <v>200</v>
+      </c>
+      <c r="B54" s="46">
+        <v>-1</v>
+      </c>
+      <c r="C54" s="46" t="s">
+        <v>211</v>
+      </c>
+      <c r="D54" s="46">
+        <v>55941</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" s="46" t="s">
+        <v>227</v>
+      </c>
+      <c r="B55" s="46"/>
+      <c r="C55" s="46" t="s">
+        <v>222</v>
+      </c>
+      <c r="D55" s="46">
+        <v>48418</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" s="46" t="s">
+        <v>202</v>
+      </c>
+      <c r="B56" s="46">
+        <v>25</v>
+      </c>
+      <c r="C56" s="46"/>
+      <c r="D56" s="46">
+        <v>-21777</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" s="46" t="s">
+        <v>225</v>
+      </c>
+      <c r="B57" s="46"/>
+      <c r="C57" s="46"/>
+      <c r="D57" s="46">
+        <v>81013</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58" s="46" t="s">
+        <v>229</v>
+      </c>
+      <c r="B58" s="46">
+        <v>29</v>
+      </c>
+      <c r="C58" s="46" t="s">
+        <v>230</v>
+      </c>
+      <c r="D58" s="46">
+        <v>-37777</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E178CC-A67A-4CEB-9ED6-E0624B3C5E2E}">
-  <dimension ref="A1:AA8"/>
+  <dimension ref="A1:AA9"/>
   <sheetViews>
     <sheetView zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
@@ -3107,20 +3872,20 @@
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21" t="s">
+      <c r="C1" s="41"/>
+      <c r="D1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="2"/>
@@ -3129,76 +3894,76 @@
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21"/>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="21"/>
-      <c r="Z1" s="21"/>
-      <c r="AA1" s="21"/>
+      <c r="T1" s="41"/>
+      <c r="U1" s="41"/>
+      <c r="V1" s="41"/>
+      <c r="W1" s="41"/>
+      <c r="X1" s="41"/>
+      <c r="Y1" s="41"/>
+      <c r="Z1" s="41"/>
+      <c r="AA1" s="41"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="20" t="s">
+      <c r="C2" s="42"/>
+      <c r="D2" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20" t="s">
+      <c r="C3" s="40"/>
+      <c r="D3" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20" t="s">
+      <c r="C4" s="40"/>
+      <c r="D4" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -3207,19 +3972,19 @@
       <c r="B5" t="s">
         <v>116</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="40" t="s">
         <v>126</v>
       </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -3228,17 +3993,17 @@
       <c r="B6" t="s">
         <v>116</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -3260,6 +4025,14 @@
       </c>
       <c r="D8" t="s">
         <v>183</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>231</v>
+      </c>
+      <c r="B9" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -3285,11 +4058,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A6F66EB-3F6A-4CB6-B201-8462253FCC87}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -3301,26 +4074,26 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="3"/>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="25" t="s">
+      <c r="C1" s="44"/>
+      <c r="D1" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="25"/>
+      <c r="E1" s="45"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20" t="s">
+      <c r="C2" s="40"/>
+      <c r="D2" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="20"/>
+      <c r="E2" s="40"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
@@ -3366,10 +4139,10 @@
       <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="20"/>
+      <c r="E8" s="40"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
@@ -3380,99 +4153,99 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="20"/>
+      <c r="C10" s="40"/>
       <c r="D10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20" t="s">
+      <c r="C11" s="40"/>
+      <c r="D11" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="E11" s="20"/>
+      <c r="E11" s="40"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="20" t="s">
+      <c r="C12" s="43"/>
+      <c r="D12" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20" t="s">
+      <c r="C13" s="40"/>
+      <c r="D13" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="E13" s="20"/>
+      <c r="E13" s="40"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>113</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>119</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20" t="s">
+      <c r="C16" s="40"/>
+      <c r="D16" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="40" t="s">
         <v>125</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20" t="s">
+      <c r="C17" s="40"/>
+      <c r="D17" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>130</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
@@ -3495,10 +4268,10 @@
       <c r="B21" t="s">
         <v>137</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="40" t="s">
         <v>138</v>
       </c>
-      <c r="E21" s="20"/>
+      <c r="E21" s="40"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
@@ -3510,6 +4283,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
     <mergeCell ref="D18:F18"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="B13:C13"/>
@@ -3521,15 +4303,6 @@
     <mergeCell ref="D16:H16"/>
     <mergeCell ref="D17:G17"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Learning Data Cleaning ( 26-7-2025 )
</commit_message>
<xml_diff>
--- a/Excel/My-Skill-Set-Track.xlsx
+++ b/Excel/My-Skill-Set-Track.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Data-Analytics\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D739EC3-FD45-4E3B-9655-454EB9723BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83CD9B8D-7F33-44A0-B379-E2B66A4A62D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{1E7A2102-239A-4535-B10C-B1AF6056B40A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="3" xr2:uid="{1E7A2102-239A-4535-B10C-B1AF6056B40A}"/>
   </bookViews>
   <sheets>
     <sheet name="Practice Problems" sheetId="8" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="212">
   <si>
     <t>Topic</t>
   </si>
@@ -615,36 +615,12 @@
     <t>Frank</t>
   </si>
   <si>
-    <t xml:space="preserve">  New York  </t>
-  </si>
-  <si>
-    <t>HANNAH</t>
-  </si>
-  <si>
     <t>Miami</t>
   </si>
   <si>
-    <t xml:space="preserve">  hannah  </t>
-  </si>
-  <si>
     <t>Los Angeles</t>
   </si>
   <si>
-    <t xml:space="preserve">  eve  </t>
-  </si>
-  <si>
-    <t>chicago</t>
-  </si>
-  <si>
-    <t>miami</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  david  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  charlie  </t>
-  </si>
-  <si>
     <t>Grace</t>
   </si>
   <si>
@@ -654,9 +630,6 @@
     <t>Hannah</t>
   </si>
   <si>
-    <t xml:space="preserve">  ivy  </t>
-  </si>
-  <si>
     <t>Jack</t>
   </si>
   <si>
@@ -666,54 +639,21 @@
     <t>Eve</t>
   </si>
   <si>
-    <t>ALICE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Atlanta  </t>
-  </si>
-  <si>
     <t>Ivy</t>
   </si>
   <si>
-    <t>boston</t>
-  </si>
-  <si>
     <t>Phoenix</t>
   </si>
   <si>
     <t>Bob</t>
   </si>
   <si>
-    <t>phoenix</t>
-  </si>
-  <si>
     <t>Seattle</t>
   </si>
   <si>
-    <t xml:space="preserve">  frank  </t>
-  </si>
-  <si>
-    <t>atlanta</t>
-  </si>
-  <si>
-    <t>JACK</t>
-  </si>
-  <si>
-    <t>Denver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Boston  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  grace  </t>
-  </si>
-  <si>
     <t>Charlie</t>
   </si>
   <si>
-    <t>denver</t>
-  </si>
-  <si>
     <t>Atlanta</t>
   </si>
   <si>
@@ -723,25 +663,22 @@
     <t>Alice</t>
   </si>
   <si>
-    <t xml:space="preserve">  jack  </t>
-  </si>
-  <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>DAVID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  bob  </t>
-  </si>
-  <si>
-    <t>houston</t>
-  </si>
-  <si>
     <t>25-7-2025</t>
   </si>
   <si>
     <t>Data Cleaning</t>
+  </si>
+  <si>
+    <t>26-7-2025</t>
+  </si>
+  <si>
+    <t>ALT+H+V+V</t>
+  </si>
+  <si>
+    <t>Paste Values</t>
+  </si>
+  <si>
+    <t>Removing Duplicates , Deleting Leading and  trailing space  TRIM() SUBSTITIUE(), Capitalize Words  PROPER(), UPPER(), LOWER(), LEN(),Handling Negative values , IF()</t>
   </si>
 </sst>
 </file>
@@ -1138,6 +1075,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1152,8 +1092,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1162,6 +1101,13 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDF240"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1176,13 +1122,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDDF240"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2220,10 +2159,10 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B2:E7">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
       <formula>40</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="greaterThan">
       <formula>80</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2287,7 +2226,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E0F8151-937B-4935-B8F3-24E8BCB42125}">
   <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
@@ -3172,7 +3111,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A2:H22">
-    <cfRule type="expression" dxfId="2" priority="10">
+    <cfRule type="expression" dxfId="0" priority="10">
       <formula>$C2="IT"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3182,671 +3121,380 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79D2C3E0-16F0-44E3-9BCD-828BC7817756}">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView zoomScale="103" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A11" zoomScale="103" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="12.36328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="47" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="40" t="s">
         <v>153</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="40" t="s">
         <v>185</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="40" t="s">
         <v>186</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="40" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46" t="s">
+      <c r="E1" s="47"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B4">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D4">
+        <v>34721</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B5">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>190</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>202</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
         <v>188</v>
       </c>
-      <c r="D2" s="46">
-        <v>60960</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="46" t="s">
+      <c r="D6">
+        <v>86833</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>193</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>197</v>
+      </c>
+      <c r="B9">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
+        <v>188</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>205</v>
+      </c>
+      <c r="B10">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>203</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>197</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>199</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>200</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>199</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>197</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>201</v>
+      </c>
+      <c r="D13">
+        <v>61024</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>189</v>
       </c>
-      <c r="B3" s="46">
-        <v>-4</v>
-      </c>
-      <c r="C3" s="46" t="s">
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>189</v>
+      </c>
+      <c r="B15">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>193</v>
+      </c>
+      <c r="D15">
+        <v>68810</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>194</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>188</v>
+      </c>
+      <c r="D16">
+        <v>52418</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>202</v>
+      </c>
+      <c r="B17">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>203</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>192</v>
+      </c>
+      <c r="B18">
+        <v>34</v>
+      </c>
+      <c r="C18" t="s">
+        <v>199</v>
+      </c>
+      <c r="D18">
+        <v>80313</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>198</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>193</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>202</v>
+      </c>
+      <c r="B20">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>204</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>200</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
         <v>190</v>
       </c>
-      <c r="D3" s="46">
-        <v>-8832</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="46" t="s">
-        <v>191</v>
-      </c>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46" t="s">
+      <c r="D21">
+        <v>56244</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>198</v>
+      </c>
+      <c r="B22">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
+        <v>204</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>195</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>193</v>
+      </c>
+      <c r="D23">
+        <v>33630</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>194</v>
+      </c>
+      <c r="B24">
+        <v>49</v>
+      </c>
+      <c r="C24" t="s">
+        <v>188</v>
+      </c>
+      <c r="D24">
+        <v>86721</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>192</v>
       </c>
-      <c r="D4" s="46">
-        <v>70288</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="46" t="s">
-        <v>193</v>
-      </c>
-      <c r="B5" s="46">
-        <v>-15</v>
-      </c>
-      <c r="C5" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="D5" s="46">
-        <v>-14166</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="B6" s="46">
-        <v>46</v>
-      </c>
-      <c r="C6" s="46" t="s">
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>199</v>
+      </c>
+      <c r="D25">
+        <v>55941</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>200</v>
+      </c>
+      <c r="B26">
+        <v>29</v>
+      </c>
+      <c r="C26" t="s">
         <v>196</v>
       </c>
-      <c r="D6" s="46">
-        <v>34721</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="46" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="46" t="s">
-        <v>193</v>
-      </c>
-      <c r="B8" s="46">
-        <v>22</v>
-      </c>
-      <c r="C8" s="46" t="s">
-        <v>197</v>
-      </c>
-      <c r="D8" s="46">
-        <v>-7809</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="46"/>
-      <c r="B9" s="46">
-        <v>-18</v>
-      </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46">
-        <v>88176</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="46" t="s">
-        <v>199</v>
-      </c>
-      <c r="B10" s="46">
-        <v>-4</v>
-      </c>
-      <c r="C10" s="46" t="s">
-        <v>188</v>
-      </c>
-      <c r="D10" s="46">
-        <v>86833</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="46" t="s">
-        <v>200</v>
-      </c>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46" t="s">
-        <v>201</v>
-      </c>
-      <c r="D11" s="46">
-        <v>-31634</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="46" t="s">
-        <v>202</v>
-      </c>
-      <c r="B12" s="46">
-        <v>-3</v>
-      </c>
-      <c r="C12" s="46" t="s">
-        <v>201</v>
-      </c>
-      <c r="D12" s="46">
-        <v>-7552</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="46" t="s">
-        <v>203</v>
-      </c>
-      <c r="B13" s="46"/>
-      <c r="C13" s="46" t="s">
-        <v>201</v>
-      </c>
-      <c r="D13" s="46">
-        <v>-49232</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="46" t="s">
-        <v>204</v>
-      </c>
-      <c r="B14" s="46">
-        <v>-16</v>
-      </c>
-      <c r="C14" s="46" t="s">
-        <v>205</v>
-      </c>
-      <c r="D14" s="46">
-        <v>-48628</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="46" t="s">
-        <v>206</v>
-      </c>
-      <c r="B15" s="46">
-        <v>46</v>
-      </c>
-      <c r="C15" s="46" t="s">
-        <v>188</v>
-      </c>
-      <c r="D15" s="46">
-        <v>-48261</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="46" t="s">
-        <v>207</v>
-      </c>
-      <c r="B16" s="46">
-        <v>28</v>
-      </c>
-      <c r="C16" s="46" t="s">
-        <v>208</v>
-      </c>
-      <c r="D16" s="46">
-        <v>-28901</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="46" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="18" spans="1:4" s="46" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="46" t="s">
-        <v>209</v>
-      </c>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46" t="s">
-        <v>210</v>
-      </c>
-      <c r="D19" s="46">
-        <v>63512</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="46" t="s">
-        <v>206</v>
-      </c>
-      <c r="B20" s="46">
-        <v>-5</v>
-      </c>
-      <c r="C20" s="46" t="s">
-        <v>211</v>
-      </c>
-      <c r="D20" s="46">
-        <v>-7670</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="46" t="s">
-        <v>212</v>
-      </c>
-      <c r="B21" s="46">
-        <v>-6</v>
-      </c>
-      <c r="C21" s="46" t="s">
-        <v>213</v>
-      </c>
-      <c r="D21" s="46">
-        <v>-30278</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="46" t="s">
-        <v>202</v>
-      </c>
-      <c r="B22" s="46">
-        <v>-12</v>
-      </c>
-      <c r="C22" s="46"/>
-      <c r="D22" s="46">
-        <v>-44867</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="46" t="s">
-        <v>212</v>
-      </c>
-      <c r="B23" s="46"/>
-      <c r="C23" s="46" t="s">
-        <v>214</v>
-      </c>
-      <c r="D23" s="46">
-        <v>55450</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="B24" s="46">
-        <v>-1</v>
-      </c>
-      <c r="C24" s="46" t="s">
-        <v>214</v>
-      </c>
-      <c r="D24" s="46">
-        <v>61024</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="46" t="s">
-        <v>189</v>
-      </c>
-      <c r="B25" s="46">
-        <v>-2</v>
-      </c>
-      <c r="C25" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="D25" s="46">
-        <v>-20466</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="46" t="s">
-        <v>215</v>
-      </c>
-      <c r="B26" s="46">
-        <v>32</v>
-      </c>
-      <c r="C26" s="46" t="s">
-        <v>201</v>
-      </c>
-      <c r="D26" s="46">
-        <v>68810</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="46" t="s">
-        <v>193</v>
-      </c>
-      <c r="B27" s="46">
-        <v>-10</v>
-      </c>
-      <c r="C27" s="46" t="s">
-        <v>188</v>
-      </c>
-      <c r="D27" s="46">
-        <v>52418</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="46" t="s">
-        <v>199</v>
-      </c>
-      <c r="B28" s="46">
-        <v>30</v>
-      </c>
-      <c r="C28" s="46" t="s">
-        <v>216</v>
-      </c>
-      <c r="D28" s="46">
-        <v>-24695</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="46" t="s">
-        <v>215</v>
-      </c>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46" t="s">
-        <v>197</v>
-      </c>
-      <c r="D29" s="46">
-        <v>66768</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="46" t="s">
-        <v>207</v>
-      </c>
-      <c r="B30" s="46">
-        <v>46</v>
-      </c>
-      <c r="C30" s="46"/>
-      <c r="D30" s="46">
-        <v>47903</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="46" t="s">
-        <v>217</v>
-      </c>
-      <c r="B31" s="46"/>
-      <c r="C31" s="46" t="s">
-        <v>218</v>
-      </c>
-      <c r="D31" s="46">
-        <v>57073</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="46" t="s">
-        <v>204</v>
-      </c>
-      <c r="B32" s="46"/>
-      <c r="C32" s="46" t="s">
-        <v>219</v>
-      </c>
-      <c r="D32" s="46">
-        <v>67004</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="46" t="s">
-        <v>220</v>
-      </c>
-      <c r="B33" s="46">
-        <v>34</v>
-      </c>
-      <c r="C33" s="46" t="s">
-        <v>213</v>
-      </c>
-      <c r="D33" s="46">
-        <v>80313</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" s="46" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="35" spans="1:4" s="46" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="46" t="s">
-        <v>203</v>
-      </c>
-      <c r="B36" s="46">
-        <v>-18</v>
-      </c>
-      <c r="C36" s="46" t="s">
-        <v>201</v>
-      </c>
-      <c r="D36" s="46">
-        <v>-29609</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="46" t="s">
-        <v>221</v>
-      </c>
-      <c r="B37" s="46">
-        <v>-17</v>
-      </c>
-      <c r="C37" s="46"/>
-      <c r="D37" s="46">
-        <v>-37817</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="46" t="s">
-        <v>206</v>
-      </c>
-      <c r="B38" s="46"/>
-      <c r="C38" s="46" t="s">
-        <v>222</v>
-      </c>
-      <c r="D38" s="46">
-        <v>-19447</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="46" t="s">
-        <v>198</v>
-      </c>
-      <c r="B39" s="46"/>
-      <c r="C39" s="46" t="s">
-        <v>223</v>
-      </c>
-      <c r="D39" s="46">
-        <v>63644</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="46" t="s">
-        <v>204</v>
-      </c>
-      <c r="B40" s="46"/>
-      <c r="C40" s="46" t="s">
-        <v>223</v>
-      </c>
-      <c r="D40" s="46">
-        <v>38532</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="46" t="s">
-        <v>189</v>
-      </c>
-      <c r="B41" s="46"/>
-      <c r="C41" s="46"/>
-      <c r="D41" s="46">
-        <v>73530</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" s="46" t="s">
-        <v>189</v>
-      </c>
-      <c r="B42" s="46"/>
-      <c r="C42" s="46" t="s">
-        <v>205</v>
-      </c>
-      <c r="D42" s="46">
-        <v>-23100</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" s="46" t="s">
-        <v>221</v>
-      </c>
-      <c r="B43" s="46">
-        <v>27</v>
-      </c>
-      <c r="C43" s="46" t="s">
-        <v>224</v>
-      </c>
-      <c r="D43" s="46">
-        <v>-37762</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" s="46" t="s">
-        <v>225</v>
-      </c>
-      <c r="B44" s="46"/>
-      <c r="C44" s="46"/>
-      <c r="D44" s="46">
-        <v>-17736</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" s="46" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" s="46" t="s">
-        <v>212</v>
-      </c>
-      <c r="B46" s="46"/>
-      <c r="C46" s="46" t="s">
-        <v>197</v>
-      </c>
-      <c r="D46" s="46">
-        <v>56244</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" s="46" t="s">
-        <v>203</v>
-      </c>
-      <c r="B47" s="46">
-        <v>30</v>
-      </c>
-      <c r="C47" s="46" t="s">
-        <v>190</v>
-      </c>
-      <c r="D47" s="46">
-        <v>-47178</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" s="46" t="s">
-        <v>226</v>
-      </c>
-      <c r="B48" s="46">
-        <v>-18</v>
-      </c>
-      <c r="C48" s="46" t="s">
-        <v>201</v>
-      </c>
-      <c r="D48" s="46">
-        <v>33630</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" s="46" t="s">
-        <v>221</v>
-      </c>
-      <c r="B49" s="46"/>
-      <c r="C49" s="46" t="s">
-        <v>216</v>
-      </c>
-      <c r="D49" s="46">
-        <v>64648</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" s="46" t="s">
-        <v>227</v>
-      </c>
-      <c r="B50" s="46"/>
-      <c r="C50" s="46" t="s">
-        <v>211</v>
-      </c>
-      <c r="D50" s="46">
-        <v>-11482</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" s="46" t="s">
-        <v>228</v>
-      </c>
-      <c r="B51" s="46"/>
-      <c r="C51" s="46" t="s">
-        <v>224</v>
-      </c>
-      <c r="D51" s="46">
-        <v>-31280</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" s="46" t="s">
-        <v>202</v>
-      </c>
-      <c r="B52" s="46">
-        <v>49</v>
-      </c>
-      <c r="C52" s="46" t="s">
-        <v>210</v>
-      </c>
-      <c r="D52" s="46">
-        <v>86721</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" s="46" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A54" s="46" t="s">
-        <v>200</v>
-      </c>
-      <c r="B54" s="46">
-        <v>-1</v>
-      </c>
-      <c r="C54" s="46" t="s">
-        <v>211</v>
-      </c>
-      <c r="D54" s="46">
-        <v>55941</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55" s="46" t="s">
-        <v>227</v>
-      </c>
-      <c r="B55" s="46"/>
-      <c r="C55" s="46" t="s">
-        <v>222</v>
-      </c>
-      <c r="D55" s="46">
-        <v>48418</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A56" s="46" t="s">
-        <v>202</v>
-      </c>
-      <c r="B56" s="46">
-        <v>25</v>
-      </c>
-      <c r="C56" s="46"/>
-      <c r="D56" s="46">
-        <v>-21777</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57" s="46" t="s">
-        <v>225</v>
-      </c>
-      <c r="B57" s="46"/>
-      <c r="C57" s="46"/>
-      <c r="D57" s="46">
-        <v>81013</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A58" s="46" t="s">
-        <v>229</v>
-      </c>
-      <c r="B58" s="46">
-        <v>29</v>
-      </c>
-      <c r="C58" s="46" t="s">
-        <v>230</v>
-      </c>
-      <c r="D58" s="46">
-        <v>-37777</v>
+      <c r="D26">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3856,36 +3504,36 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E178CC-A67A-4CEB-9ED6-E0624B3C5E2E}">
-  <dimension ref="A1:AA9"/>
+  <dimension ref="A1:AA10"/>
   <sheetViews>
-    <sheetView zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.54296875" customWidth="1"/>
-    <col min="4" max="4" width="95.6328125" customWidth="1"/>
+    <col min="4" max="4" width="115.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41" t="s">
+      <c r="C1" s="42"/>
+      <c r="D1" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="2"/>
@@ -3894,76 +3542,76 @@
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
-      <c r="T1" s="41"/>
-      <c r="U1" s="41"/>
-      <c r="V1" s="41"/>
-      <c r="W1" s="41"/>
-      <c r="X1" s="41"/>
-      <c r="Y1" s="41"/>
-      <c r="Z1" s="41"/>
-      <c r="AA1" s="41"/>
+      <c r="T1" s="42"/>
+      <c r="U1" s="42"/>
+      <c r="V1" s="42"/>
+      <c r="W1" s="42"/>
+      <c r="X1" s="42"/>
+      <c r="Y1" s="42"/>
+      <c r="Z1" s="42"/>
+      <c r="AA1" s="42"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="40" t="s">
+      <c r="C2" s="43"/>
+      <c r="D2" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40" t="s">
+      <c r="C3" s="41"/>
+      <c r="D3" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40" t="s">
+      <c r="C4" s="41"/>
+      <c r="D4" s="41" t="s">
         <v>117</v>
       </c>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -3972,19 +3620,19 @@
       <c r="B5" t="s">
         <v>116</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="41" t="s">
         <v>126</v>
       </c>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="40"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="41"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -3993,17 +3641,17 @@
       <c r="B6" t="s">
         <v>116</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="41" t="s">
         <v>144</v>
       </c>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -4029,14 +3677,28 @@
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>231</v>
+        <v>206</v>
       </c>
       <c r="B9" t="s">
-        <v>232</v>
-      </c>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>208</v>
+      </c>
+      <c r="B10" t="s">
+        <v>207</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>211</v>
+      </c>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
+    <mergeCell ref="D10:F10"/>
     <mergeCell ref="D6:L6"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:J4"/>
@@ -4060,10 +3722,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A6F66EB-3F6A-4CB6-B201-8462253FCC87}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D17" sqref="D17:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4074,26 +3736,26 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="3"/>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="45" t="s">
+      <c r="C1" s="45"/>
+      <c r="D1" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="45"/>
+      <c r="E1" s="46"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40" t="s">
+      <c r="C2" s="41"/>
+      <c r="D2" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="40"/>
+      <c r="E2" s="41"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
@@ -4139,10 +3801,10 @@
       <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="40"/>
+      <c r="E8" s="41"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
@@ -4153,99 +3815,99 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="40"/>
+      <c r="C10" s="41"/>
       <c r="D10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="41" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40" t="s">
+      <c r="C11" s="41"/>
+      <c r="D11" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="E11" s="40"/>
+      <c r="E11" s="41"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="44" t="s">
         <v>109</v>
       </c>
-      <c r="C12" s="43"/>
-      <c r="D12" s="40" t="s">
+      <c r="C12" s="44"/>
+      <c r="D12" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40" t="s">
+      <c r="C13" s="41"/>
+      <c r="D13" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="E13" s="40"/>
+      <c r="E13" s="41"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>113</v>
       </c>
-      <c r="D14" s="40" t="s">
+      <c r="D14" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>119</v>
       </c>
-      <c r="D15" s="40" t="s">
+      <c r="D15" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40" t="s">
+      <c r="C16" s="41"/>
+      <c r="D16" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40" t="s">
+      <c r="C17" s="41"/>
+      <c r="D17" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>130</v>
       </c>
-      <c r="D18" s="40" t="s">
+      <c r="D18" s="41" t="s">
         <v>131</v>
       </c>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
@@ -4268,10 +3930,10 @@
       <c r="B21" t="s">
         <v>137</v>
       </c>
-      <c r="D21" s="40" t="s">
+      <c r="D21" s="41" t="s">
         <v>138</v>
       </c>
-      <c r="E21" s="40"/>
+      <c r="E21" s="41"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
@@ -4281,17 +3943,16 @@
         <v>152</v>
       </c>
     </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>209</v>
+      </c>
+      <c r="D23" t="s">
+        <v>210</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
     <mergeCell ref="D18:F18"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="B13:C13"/>
@@ -4303,6 +3964,15 @@
     <mergeCell ref="D16:H16"/>
     <mergeCell ref="D17:G17"/>
     <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Studying Data Split (28-7-2025 )
</commit_message>
<xml_diff>
--- a/Excel/My-Skill-Set-Track.xlsx
+++ b/Excel/My-Skill-Set-Track.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Data-Analytics\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83CD9B8D-7F33-44A0-B379-E2B66A4A62D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD26E095-E4D7-41C5-8711-1C7B3F563306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="3" xr2:uid="{1E7A2102-239A-4535-B10C-B1AF6056B40A}"/>
   </bookViews>
@@ -16,11 +16,12 @@
     <sheet name="Practice Problems" sheetId="8" r:id="rId1"/>
     <sheet name="Data Entry" sheetId="6" r:id="rId2"/>
     <sheet name="Data Cleaning" sheetId="9" r:id="rId3"/>
-    <sheet name="Track" sheetId="1" r:id="rId4"/>
-    <sheet name="Shorcut Keys" sheetId="7" r:id="rId5"/>
+    <sheet name="Data Split" sheetId="10" r:id="rId4"/>
+    <sheet name="Track" sheetId="1" r:id="rId5"/>
+    <sheet name="Shorcut Keys" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">Track!$A$1:$AA$3</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">Track!$A$1:$AA$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="218">
   <si>
     <t>Topic</t>
   </si>
@@ -679,6 +680,24 @@
   </si>
   <si>
     <t>Removing Duplicates , Deleting Leading and  trailing space  TRIM() SUBSTITIUE(), Capitalize Words  PROPER(), UPPER(), LOWER(), LEN(),Handling Negative values , IF()</t>
+  </si>
+  <si>
+    <t>City-Pin</t>
+  </si>
+  <si>
+    <t>Badin-72200</t>
+  </si>
+  <si>
+    <t>Karachi-44220</t>
+  </si>
+  <si>
+    <t>Hyderabad-33002</t>
+  </si>
+  <si>
+    <t>Lahore-22110</t>
+  </si>
+  <si>
+    <t>Islamabad-33229</t>
   </si>
 </sst>
 </file>
@@ -1078,6 +1097,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1091,9 +1113,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3145,7 +3164,7 @@
       <c r="D1" s="40" t="s">
         <v>187</v>
       </c>
-      <c r="E1" s="47"/>
+      <c r="E1" s="41"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -3503,10 +3522,55 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE157058-8853-4CE4-B4AD-54BF043BDEFE}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E178CC-A67A-4CEB-9ED6-E0624B3C5E2E}">
   <dimension ref="A1:AA10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
+    <sheetView zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -3520,20 +3584,20 @@
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42" t="s">
+      <c r="C1" s="43"/>
+      <c r="D1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="2"/>
@@ -3542,76 +3606,76 @@
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
-      <c r="T1" s="42"/>
-      <c r="U1" s="42"/>
-      <c r="V1" s="42"/>
-      <c r="W1" s="42"/>
-      <c r="X1" s="42"/>
-      <c r="Y1" s="42"/>
-      <c r="Z1" s="42"/>
-      <c r="AA1" s="42"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="43"/>
+      <c r="X1" s="43"/>
+      <c r="Y1" s="43"/>
+      <c r="Z1" s="43"/>
+      <c r="AA1" s="43"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="41" t="s">
+      <c r="C2" s="44"/>
+      <c r="D2" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41" t="s">
+      <c r="C3" s="42"/>
+      <c r="D3" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41" t="s">
+      <c r="C4" s="42"/>
+      <c r="D4" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -3620,19 +3684,19 @@
       <c r="B5" t="s">
         <v>116</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="41"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
+      <c r="N5" s="42"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -3641,17 +3705,17 @@
       <c r="B6" t="s">
         <v>116</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="41"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="42"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -3690,29 +3754,29 @@
       <c r="B10" t="s">
         <v>207</v>
       </c>
-      <c r="D10" s="41" t="s">
+      <c r="D10" s="42" t="s">
         <v>211</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:K1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:N3"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="D2:N2"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="X1:Y1"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="D6:L6"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:J4"/>
     <mergeCell ref="D5:N5"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="D2:N2"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:K1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:N3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3720,7 +3784,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A6F66EB-3F6A-4CB6-B201-8462253FCC87}">
   <dimension ref="A1:H23"/>
   <sheetViews>
@@ -3736,26 +3800,26 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="3"/>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="46" t="s">
+      <c r="C1" s="46"/>
+      <c r="D1" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="46"/>
+      <c r="E1" s="47"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41" t="s">
+      <c r="C2" s="42"/>
+      <c r="D2" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="41"/>
+      <c r="E2" s="42"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
@@ -3801,10 +3865,10 @@
       <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="41" t="s">
+      <c r="D8" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="41"/>
+      <c r="E8" s="42"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
@@ -3815,99 +3879,99 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="41"/>
+      <c r="C10" s="42"/>
       <c r="D10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="42" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41" t="s">
+      <c r="C11" s="42"/>
+      <c r="D11" s="42" t="s">
         <v>102</v>
       </c>
-      <c r="E11" s="41"/>
+      <c r="E11" s="42"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="41" t="s">
+      <c r="C12" s="45"/>
+      <c r="D12" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41" t="s">
+      <c r="C13" s="42"/>
+      <c r="D13" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="E13" s="41"/>
+      <c r="E13" s="42"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>113</v>
       </c>
-      <c r="D14" s="41" t="s">
+      <c r="D14" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>119</v>
       </c>
-      <c r="D15" s="41" t="s">
+      <c r="D15" s="42" t="s">
         <v>120</v>
       </c>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41" t="s">
+      <c r="C16" s="42"/>
+      <c r="D16" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41" t="s">
+      <c r="C17" s="42"/>
+      <c r="D17" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>130</v>
       </c>
-      <c r="D18" s="41" t="s">
+      <c r="D18" s="42" t="s">
         <v>131</v>
       </c>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
@@ -3930,10 +3994,10 @@
       <c r="B21" t="s">
         <v>137</v>
       </c>
-      <c r="D21" s="41" t="s">
+      <c r="D21" s="42" t="s">
         <v>138</v>
       </c>
-      <c r="E21" s="41"/>
+      <c r="E21" s="42"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
@@ -3953,6 +4017,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
     <mergeCell ref="D18:F18"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="B13:C13"/>
@@ -3964,15 +4037,6 @@
     <mergeCell ref="D16:H16"/>
     <mergeCell ref="D17:G17"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Learning Data Split (29-7-2025 )
</commit_message>
<xml_diff>
--- a/Excel/My-Skill-Set-Track.xlsx
+++ b/Excel/My-Skill-Set-Track.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Data-Analytics\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD26E095-E4D7-41C5-8711-1C7B3F563306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197932A5-730D-43AB-AEA8-26A64FDC5F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="3" xr2:uid="{1E7A2102-239A-4535-B10C-B1AF6056B40A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="4" xr2:uid="{1E7A2102-239A-4535-B10C-B1AF6056B40A}"/>
   </bookViews>
   <sheets>
     <sheet name="Practice Problems" sheetId="8" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="219">
   <si>
     <t>Topic</t>
   </si>
@@ -698,6 +698,9 @@
   </si>
   <si>
     <t>Islamabad-33229</t>
+  </si>
+  <si>
+    <t>29-7-2025</t>
   </si>
 </sst>
 </file>
@@ -3142,7 +3145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79D2C3E0-16F0-44E3-9BCD-828BC7817756}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="103" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="103" workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -3525,7 +3528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE157058-8853-4CE4-B4AD-54BF043BDEFE}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -3568,15 +3571,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E178CC-A67A-4CEB-9ED6-E0624B3C5E2E}">
-  <dimension ref="A1:AA10"/>
+  <dimension ref="A1:AA11"/>
   <sheetViews>
-    <sheetView zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.54296875" customWidth="1"/>
+    <col min="2" max="2" width="16.90625" customWidth="1"/>
     <col min="4" max="4" width="115.81640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3759,6 +3763,11 @@
       </c>
       <c r="E10" s="42"/>
       <c r="F10" s="42"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>218</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>

<commit_message>
Learning Data Split (5-8-2025 )
</commit_message>
<xml_diff>
--- a/Excel/My-Skill-Set-Track.xlsx
+++ b/Excel/My-Skill-Set-Track.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Data-Analytics\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197932A5-730D-43AB-AEA8-26A64FDC5F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876C7412-40EF-4E85-82D7-04C4A24576F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="4" xr2:uid="{1E7A2102-239A-4535-B10C-B1AF6056B40A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="3" xr2:uid="{1E7A2102-239A-4535-B10C-B1AF6056B40A}"/>
   </bookViews>
   <sheets>
     <sheet name="Practice Problems" sheetId="8" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="223">
   <si>
     <t>Topic</t>
   </si>
@@ -700,16 +700,29 @@
     <t>Islamabad-33229</t>
   </si>
   <si>
-    <t>29-7-2025</t>
+    <t>CTRL+E</t>
+  </si>
+  <si>
+    <t>Pin</t>
+  </si>
+  <si>
+    <t>Flash Fill ( for data split)</t>
+  </si>
+  <si>
+    <t>Data Split</t>
+  </si>
+  <si>
+    <t>Split data using flash fill</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="dd\-mmm\-yyyy"/>
+    <numFmt numFmtId="169" formatCode="dd/m/yyyy"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -1030,7 +1043,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1103,13 +1116,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1117,6 +1130,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="169" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -3526,42 +3541,101 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE157058-8853-4CE4-B4AD-54BF043BDEFE}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.1796875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2">
+        <v>72200</v>
+      </c>
+      <c r="E2" t="str">
+        <f>LEFT(A2,FIND("-",A2,1)-1)</f>
+        <v>Badin</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3">
+        <v>44220</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E6" si="0">LEFT(A3,FIND("-",A3,1)-1)</f>
+        <v>Karachi</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4">
+        <v>33002</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>Hyderabad</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5">
+        <v>22110</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>Lahore</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>217</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6">
+        <v>33229</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>Islamabad</v>
       </c>
     </row>
   </sheetData>
@@ -3573,35 +3647,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E178CC-A67A-4CEB-9ED6-E0624B3C5E2E}">
   <dimension ref="A1:AA11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" style="49" customWidth="1"/>
     <col min="2" max="2" width="16.90625" customWidth="1"/>
     <col min="4" max="4" width="115.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43" t="s">
+      <c r="C1" s="42"/>
+      <c r="D1" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="2"/>
@@ -3610,119 +3684,119 @@
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
-      <c r="T1" s="43"/>
-      <c r="U1" s="43"/>
-      <c r="V1" s="43"/>
-      <c r="W1" s="43"/>
-      <c r="X1" s="43"/>
-      <c r="Y1" s="43"/>
-      <c r="Z1" s="43"/>
-      <c r="AA1" s="43"/>
+      <c r="T1" s="42"/>
+      <c r="U1" s="42"/>
+      <c r="V1" s="42"/>
+      <c r="W1" s="42"/>
+      <c r="X1" s="42"/>
+      <c r="Y1" s="42"/>
+      <c r="Z1" s="42"/>
+      <c r="AA1" s="42"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="42" t="s">
+      <c r="C2" s="43"/>
+      <c r="D2" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="42"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42" t="s">
+      <c r="C3" s="44"/>
+      <c r="D3" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="49" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="44" t="s">
         <v>116</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42" t="s">
+      <c r="C4" s="44"/>
+      <c r="D4" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="49" t="s">
         <v>118</v>
       </c>
       <c r="B5" t="s">
         <v>116</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="42"/>
-      <c r="N5" s="42"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="44"/>
+      <c r="N5" s="44"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="49" t="s">
         <v>139</v>
       </c>
       <c r="B6" t="s">
         <v>116</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="44" t="s">
         <v>144</v>
       </c>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="42"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="44"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="49" t="s">
         <v>145</v>
       </c>
       <c r="B7" t="s">
@@ -3733,7 +3807,7 @@
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" s="49" t="s">
         <v>181</v>
       </c>
       <c r="B8" t="s">
@@ -3744,7 +3818,7 @@
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="A9" s="49" t="s">
         <v>206</v>
       </c>
       <c r="B9" t="s">
@@ -3752,40 +3826,46 @@
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="A10" s="49" t="s">
         <v>208</v>
       </c>
       <c r="B10" t="s">
         <v>207</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="44" t="s">
         <v>211</v>
       </c>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>218</v>
+      <c r="A11" s="49">
+        <v>45785</v>
+      </c>
+      <c r="B11" t="s">
+        <v>221</v>
+      </c>
+      <c r="D11" t="s">
+        <v>222</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D6:L6"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:J4"/>
+    <mergeCell ref="D5:N5"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="D2:N2"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="X1:Y1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:K1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D3:N3"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="D2:N2"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D6:L6"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:J4"/>
-    <mergeCell ref="D5:N5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3795,10 +3875,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A6F66EB-3F6A-4CB6-B201-8462253FCC87}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:G17"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3821,14 +3901,14 @@
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42" t="s">
+      <c r="C2" s="44"/>
+      <c r="D2" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="42"/>
+      <c r="E2" s="44"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
@@ -3874,10 +3954,10 @@
       <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="42"/>
+      <c r="E8" s="44"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
@@ -3888,99 +3968,99 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="42"/>
+      <c r="C10" s="44"/>
       <c r="D10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="44" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42" t="s">
+      <c r="C11" s="44"/>
+      <c r="D11" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="E11" s="42"/>
+      <c r="E11" s="44"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B12" s="45" t="s">
         <v>109</v>
       </c>
       <c r="C12" s="45"/>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="44" t="s">
         <v>110</v>
       </c>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42" t="s">
+      <c r="C13" s="44"/>
+      <c r="D13" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="E13" s="42"/>
+      <c r="E13" s="44"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>113</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>119</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="44" t="s">
         <v>120</v>
       </c>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42" t="s">
+      <c r="C16" s="44"/>
+      <c r="D16" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42" t="s">
+      <c r="C17" s="44"/>
+      <c r="D17" s="44" t="s">
         <v>124</v>
       </c>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>130</v>
       </c>
-      <c r="D18" s="42" t="s">
+      <c r="D18" s="44" t="s">
         <v>131</v>
       </c>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
@@ -4003,10 +4083,10 @@
       <c r="B21" t="s">
         <v>137</v>
       </c>
-      <c r="D21" s="42" t="s">
+      <c r="D21" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="E21" s="42"/>
+      <c r="E21" s="44"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
@@ -4024,17 +4104,16 @@
         <v>210</v>
       </c>
     </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>218</v>
+      </c>
+      <c r="D24" t="s">
+        <v>220</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
     <mergeCell ref="D18:F18"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="B13:C13"/>
@@ -4046,6 +4125,15 @@
     <mergeCell ref="D16:H16"/>
     <mergeCell ref="D17:G17"/>
     <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Learning Data Split (9-8-2025 )
</commit_message>
<xml_diff>
--- a/Excel/My-Skill-Set-Track.xlsx
+++ b/Excel/My-Skill-Set-Track.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Data-Analytics\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876C7412-40EF-4E85-82D7-04C4A24576F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CCAC4A-6C1B-4733-BB09-34C91BC68B8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="3" xr2:uid="{1E7A2102-239A-4535-B10C-B1AF6056B40A}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10890" firstSheet="2" activeTab="3" xr2:uid="{1E7A2102-239A-4535-B10C-B1AF6056B40A}"/>
   </bookViews>
   <sheets>
     <sheet name="Practice Problems" sheetId="8" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="216">
   <si>
     <t>Topic</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Decription</t>
   </si>
   <si>
-    <t>16-7-2025</t>
-  </si>
-  <si>
     <t>Excel Basics</t>
   </si>
   <si>
@@ -103,9 +100,6 @@
     <t>Open Workbook</t>
   </si>
   <si>
-    <t>18-7-2025</t>
-  </si>
-  <si>
     <t>SUM function, Password Protection on Worksheets and Workbooks</t>
   </si>
   <si>
@@ -391,18 +385,12 @@
     <t>DialogBox to chose what to add</t>
   </si>
   <si>
-    <t>20-7-2025</t>
-  </si>
-  <si>
     <t>Data Entry</t>
   </si>
   <si>
     <t xml:space="preserve">Fill handle, Filling Columns , adding Columns , row , Deleting Columns , rows  </t>
   </si>
   <si>
-    <t xml:space="preserve">21-7-2025 </t>
-  </si>
-  <si>
     <t>CTRL+1</t>
   </si>
   <si>
@@ -463,9 +451,6 @@
     <t>To Fix Value in Formula</t>
   </si>
   <si>
-    <t xml:space="preserve">22-7-2025 </t>
-  </si>
-  <si>
     <t>MAX</t>
   </si>
   <si>
@@ -481,9 +466,6 @@
     <t>SUM Formula , adding marks ,paste values, fix refrence , relative refrence,MAX,MIN,AVG,COUNT</t>
   </si>
   <si>
-    <t>23-7-2025</t>
-  </si>
-  <si>
     <t xml:space="preserve">Conditional Formating,Advance Conditional Formating </t>
   </si>
   <si>
@@ -589,9 +571,6 @@
     <t>Urdu</t>
   </si>
   <si>
-    <t xml:space="preserve">24-7-2025 </t>
-  </si>
-  <si>
     <t xml:space="preserve">Practice </t>
   </si>
   <si>
@@ -664,15 +643,9 @@
     <t>Alice</t>
   </si>
   <si>
-    <t>25-7-2025</t>
-  </si>
-  <si>
     <t>Data Cleaning</t>
   </si>
   <si>
-    <t>26-7-2025</t>
-  </si>
-  <si>
     <t>ALT+H+V+V</t>
   </si>
   <si>
@@ -713,6 +686,12 @@
   </si>
   <si>
     <t>Split data using flash fill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Split </t>
+  </si>
+  <si>
+    <t>LEFT(),RIGHT(),FIND()</t>
   </si>
 </sst>
 </file>
@@ -722,7 +701,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="dd\-mmm\-yyyy"/>
-    <numFmt numFmtId="169" formatCode="dd/m/yyyy"/>
+    <numFmt numFmtId="171" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -1116,13 +1095,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1130,8 +1109,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1805,45 +1784,45 @@
   <sheetData>
     <row r="1" spans="1:15" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="16" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>160</v>
-      </c>
       <c r="G1" s="16" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="K1" s="16" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="M1" s="16" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B2" s="24">
         <v>78</v>
@@ -1884,12 +1863,12 @@
         <v>45658</v>
       </c>
       <c r="O2" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="31" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B3" s="17">
         <v>65</v>
@@ -1930,12 +1909,12 @@
         <v>45658</v>
       </c>
       <c r="O3" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="31" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B4" s="17">
         <v>90</v>
@@ -1976,12 +1955,12 @@
         <v>45658</v>
       </c>
       <c r="O4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="31" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B5" s="17">
         <v>64</v>
@@ -2022,12 +2001,12 @@
         <v>45658</v>
       </c>
       <c r="O5" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="31" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B6" s="17">
         <v>84</v>
@@ -2068,12 +2047,12 @@
         <v>45658</v>
       </c>
       <c r="O6" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="33" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B7" s="34">
         <v>43</v>
@@ -2114,48 +2093,48 @@
         <v>45658</v>
       </c>
       <c r="O7" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="O8" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="O9" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="O10" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="O11" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="O12" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="O13" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D15" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="E15" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
@@ -2281,51 +2260,51 @@
   <sheetData>
     <row r="1" spans="1:19" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D1" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>28</v>
-      </c>
       <c r="F1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="8" t="s">
-        <v>29</v>
-      </c>
       <c r="H1" s="10" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D2" s="13">
         <v>38000</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F2" s="6">
         <v>20</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H2" s="11">
         <v>45661</v>
@@ -2333,25 +2312,25 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D3" s="13">
         <v>36000</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F3" s="6">
         <v>21</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H3" s="11">
         <v>45662</v>
@@ -2359,25 +2338,25 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D4" s="13">
         <v>34000</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F4" s="6">
         <v>21</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H4" s="11">
         <v>45663</v>
@@ -2385,25 +2364,25 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D5" s="13">
         <v>32000</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F5" s="6">
         <v>20</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H5" s="11">
         <v>45664</v>
@@ -2411,75 +2390,75 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D6" s="13">
         <v>30000</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F6" s="6">
         <v>23</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H6" s="11">
         <v>45665</v>
       </c>
       <c r="L6" s="15" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="M6" s="15" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="N6" s="15" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="O6" s="15" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="P6" s="15" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="Q6" s="15" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="R6" s="15" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="S6" s="15" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D7" s="13">
         <v>28000</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F7" s="6">
         <v>24</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H7" s="11">
         <v>45666</v>
@@ -2516,25 +2495,25 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D8" s="13">
         <v>26000</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F8" s="6">
         <v>23</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H8" s="11">
         <v>45667</v>
@@ -2571,25 +2550,25 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D9" s="13">
         <v>24000</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F9" s="6">
         <v>26</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H9" s="11">
         <v>45668</v>
@@ -2626,25 +2605,25 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D10" s="13">
         <v>22000</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F10" s="6">
         <v>28</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H10" s="11">
         <v>45669</v>
@@ -2681,25 +2660,25 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D11" s="13">
         <v>20000</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F11" s="6">
         <v>30</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H11" s="11">
         <v>45670</v>
@@ -2736,25 +2715,25 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D12" s="13">
         <v>18000</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F12" s="6">
         <v>20</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H12" s="11">
         <v>45671</v>
@@ -2791,25 +2770,25 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D13" s="13">
         <v>16000</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F13" s="6">
         <v>23</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H13" s="11">
         <v>45672</v>
@@ -2846,25 +2825,25 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D14" s="13">
         <v>14000</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F14" s="6">
         <v>21</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H14" s="11">
         <v>45673</v>
@@ -2901,25 +2880,25 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D15" s="13">
         <v>12000</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F15" s="6">
         <v>25</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H15" s="11">
         <v>45674</v>
@@ -2956,25 +2935,25 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D16" s="13">
         <v>10000</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F16" s="6">
         <v>25</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H16" s="11">
         <v>45675</v>
@@ -3011,25 +2990,25 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D17" s="13">
         <v>8000</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F17" s="6">
         <v>21</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H17" s="11">
         <v>45676</v>
@@ -3037,25 +3016,25 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D18" s="13">
         <v>6000</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F18" s="6">
         <v>20</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H18" s="11">
         <v>45677</v>
@@ -3063,25 +3042,25 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D19" s="13">
         <v>4000</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F19" s="6">
         <v>20</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H19" s="11">
         <v>45678</v>
@@ -3092,25 +3071,25 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D20" s="13">
         <v>2000</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F20" s="6">
         <v>20</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H20" s="11">
         <v>45679</v>
@@ -3118,28 +3097,28 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D21" s="13">
         <v>2000</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F21" s="6">
         <v>28</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
@@ -3160,8 +3139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79D2C3E0-16F0-44E3-9BCD-828BC7817756}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="103" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView zoomScale="103" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3171,28 +3150,28 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="40" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="E1" s="41"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -3200,13 +3179,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -3214,13 +3193,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B4">
         <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="D4">
         <v>34721</v>
@@ -3228,13 +3207,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="B5">
         <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -3242,13 +3221,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="D6">
         <v>86833</v>
@@ -3256,13 +3235,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -3270,13 +3249,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -3284,13 +3263,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B9">
         <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -3298,13 +3277,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="B10">
         <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -3312,13 +3291,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -3326,13 +3305,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -3340,13 +3319,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="D13">
         <v>61024</v>
@@ -3354,13 +3333,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -3368,13 +3347,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B15">
         <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="D15">
         <v>68810</v>
@@ -3382,13 +3361,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="D16">
         <v>52418</v>
@@ -3396,13 +3375,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="B17">
         <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -3410,13 +3389,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="B18">
         <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="D18">
         <v>80313</v>
@@ -3424,13 +3403,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -3438,13 +3417,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="B20">
         <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -3452,13 +3431,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="D21">
         <v>56244</v>
@@ -3466,13 +3445,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B22">
         <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -3480,13 +3459,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="B23">
         <v>0</v>
       </c>
       <c r="C23" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="D23">
         <v>33630</v>
@@ -3494,13 +3473,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="B24">
         <v>49</v>
       </c>
       <c r="C24" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="D24">
         <v>86721</v>
@@ -3508,13 +3487,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="B25">
         <v>0</v>
       </c>
       <c r="C25" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="D25">
         <v>55941</v>
@@ -3522,13 +3501,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B26">
         <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -3541,34 +3520,35 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE157058-8853-4CE4-B4AD-54BF043BDEFE}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22.1796875" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="B1" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="C1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C2">
         <v>72200</v>
@@ -3577,13 +3557,17 @@
         <f>LEFT(A2,FIND("-",A2,1)-1)</f>
         <v>Badin</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2" t="str">
+        <f>RIGHT(A2,LEN(A2)-FIND("-",A2,1))</f>
+        <v>72200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C3">
         <v>44220</v>
@@ -3592,13 +3576,17 @@
         <f t="shared" ref="E3:E6" si="0">LEFT(A3,FIND("-",A3,1)-1)</f>
         <v>Karachi</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F6" si="1">RIGHT(A3,LEN(A3)-FIND("-",A3,1))</f>
+        <v>44220</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C4">
         <v>33002</v>
@@ -3607,13 +3595,17 @@
         <f t="shared" si="0"/>
         <v>Hyderabad</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4" t="str">
+        <f t="shared" si="1"/>
+        <v>33002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C5">
         <v>22110</v>
@@ -3622,13 +3614,17 @@
         <f t="shared" si="0"/>
         <v>Lahore</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5" t="str">
+        <f t="shared" si="1"/>
+        <v>22110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C6">
         <v>33229</v>
@@ -3636,6 +3632,10 @@
       <c r="E6" t="str">
         <f t="shared" si="0"/>
         <v>Islamabad</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="1"/>
+        <v>33229</v>
       </c>
     </row>
   </sheetData>
@@ -3645,37 +3645,37 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E178CC-A67A-4CEB-9ED6-E0624B3C5E2E}">
-  <dimension ref="A1:AA11"/>
+  <dimension ref="A1:AA12"/>
   <sheetViews>
     <sheetView zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" style="49" customWidth="1"/>
+    <col min="1" max="1" width="12.08984375" style="9" customWidth="1"/>
     <col min="2" max="2" width="16.90625" customWidth="1"/>
     <col min="4" max="4" width="115.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A1" s="48" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="42" t="s">
+      <c r="A1" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42" t="s">
+      <c r="C1" s="43"/>
+      <c r="D1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="2"/>
@@ -3684,188 +3684,199 @@
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
-      <c r="T1" s="42"/>
-      <c r="U1" s="42"/>
-      <c r="V1" s="42"/>
-      <c r="W1" s="42"/>
-      <c r="X1" s="42"/>
-      <c r="Y1" s="42"/>
-      <c r="Z1" s="42"/>
-      <c r="AA1" s="42"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="43"/>
+      <c r="X1" s="43"/>
+      <c r="Y1" s="43"/>
+      <c r="Z1" s="43"/>
+      <c r="AA1" s="43"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="48">
+        <v>45854</v>
+      </c>
+      <c r="B2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A3" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="44" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
+      <c r="A3" s="48">
+        <v>45856</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A4" s="49" t="s">
-        <v>115</v>
-      </c>
-      <c r="B4" s="44" t="s">
-        <v>116</v>
-      </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44" t="s">
-        <v>117</v>
-      </c>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
+      <c r="A4" s="48">
+        <v>45858</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A5" s="49" t="s">
-        <v>118</v>
+      <c r="A5" s="48">
+        <v>45859</v>
       </c>
       <c r="B5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D5" s="44" t="s">
-        <v>126</v>
-      </c>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="44"/>
-      <c r="N5" s="44"/>
+        <v>113</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
+      <c r="N5" s="42"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="48">
+        <v>45860</v>
+      </c>
+      <c r="B6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" s="42" t="s">
         <v>139</v>
       </c>
-      <c r="B6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D6" s="44" t="s">
-        <v>144</v>
-      </c>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="44"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="42"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A7" s="49" t="s">
-        <v>145</v>
+      <c r="A7" s="48">
+        <v>45861</v>
       </c>
       <c r="B7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D7" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A8" s="49" t="s">
-        <v>181</v>
+      <c r="A8" s="48">
+        <v>45862</v>
       </c>
       <c r="B8" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="D8" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A9" s="49" t="s">
-        <v>206</v>
+      <c r="A9" s="48">
+        <v>45863</v>
       </c>
       <c r="B9" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A10" s="49" t="s">
-        <v>208</v>
+      <c r="A10" s="48">
+        <v>45864</v>
       </c>
       <c r="B10" t="s">
-        <v>207</v>
-      </c>
-      <c r="D10" s="44" t="s">
-        <v>211</v>
-      </c>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
+        <v>199</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>202</v>
+      </c>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A11" s="49">
-        <v>45785</v>
+      <c r="A11" s="48">
+        <v>45874</v>
       </c>
       <c r="B11" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="D11" t="s">
-        <v>222</v>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A12" s="48">
+        <v>45908</v>
+      </c>
+      <c r="B12" t="s">
+        <v>214</v>
+      </c>
+      <c r="D12" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:K1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:N3"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="D2:N2"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="X1:Y1"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="D6:L6"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:J4"/>
     <mergeCell ref="D5:N5"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="D2:N2"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:K1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:N3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3877,7 +3888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A6F66EB-3F6A-4CB6-B201-8462253FCC87}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -3890,230 +3901,239 @@
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="3"/>
       <c r="B1" s="46" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C1" s="46"/>
       <c r="D1" s="47" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" s="47"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="44"/>
+      <c r="E2" s="42"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
         <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
         <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="44"/>
+      <c r="E8" s="42"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
         <v>23</v>
       </c>
-      <c r="D9" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B10" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="44"/>
+      <c r="B10" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="42"/>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B11" s="44" t="s">
-        <v>101</v>
-      </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44" t="s">
-        <v>102</v>
-      </c>
-      <c r="E11" s="44"/>
+      <c r="B11" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="E11" s="42"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B12" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="45"/>
+      <c r="D12" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="C12" s="45"/>
-      <c r="D12" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44" t="s">
-        <v>112</v>
-      </c>
-      <c r="E13" s="44"/>
+      <c r="E13" s="42"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>113</v>
-      </c>
-      <c r="D14" s="44" t="s">
-        <v>114</v>
-      </c>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
+        <v>111</v>
+      </c>
+      <c r="D14" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
+        <v>115</v>
+      </c>
+      <c r="D15" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B16" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="D15" s="44" t="s">
+      <c r="C16" s="42"/>
+      <c r="D16" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B17" s="42" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42" t="s">
         <v>120</v>
       </c>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B16" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44" t="s">
-        <v>122</v>
-      </c>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B17" s="44" t="s">
-        <v>125</v>
-      </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44" t="s">
-        <v>124</v>
-      </c>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>130</v>
-      </c>
-      <c r="D18" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="E18" s="44"/>
-      <c r="F18" s="44"/>
+        <v>126</v>
+      </c>
+      <c r="D18" s="42" t="s">
+        <v>127</v>
+      </c>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D19" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D20" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>137</v>
-      </c>
-      <c r="D21" s="44" t="s">
-        <v>138</v>
-      </c>
-      <c r="E21" s="44"/>
+        <v>133</v>
+      </c>
+      <c r="D21" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="E21" s="42"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D22" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="D23" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="D24" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
     <mergeCell ref="D18:F18"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="B13:C13"/>
@@ -4125,15 +4145,6 @@
     <mergeCell ref="D16:H16"/>
     <mergeCell ref="D17:G17"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>